<commit_message>
Improve plot_timeseries_indicator and Fix issues raised by new `scenario` structure
</commit_message>
<xml_diff>
--- a/inst/extdata/test_scenarios_uhc_afg.xlsx
+++ b/inst/extdata/test_scenarios_uhc_afg.xlsx
@@ -1770,7 +1770,7 @@
     <t>Raw values *</t>
   </si>
   <si>
-    <t xml:space="preserve">Date Summary Generated: 2022-01-26</t>
+    <t xml:space="preserve">Date Summary Generated: 2022-03-07</t>
   </si>
   <si>
     <t xml:space="preserve">Billion</t>
@@ -2229,17 +2229,17 @@
     <t xml:space="preserve">default</t>
   </si>
   <si>
-    <t xml:space="preserve">acceleration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">halt_rise</t>
+    <t xml:space="preserve">covid_dip_lag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pre_covid_trajectory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="199">
+  <numFmts count="209">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="TXT"/>
     <numFmt numFmtId="167" formatCode="TXT"/>
@@ -2373,10 +2373,10 @@
     <numFmt numFmtId="295" formatCode="0.00"/>
     <numFmt numFmtId="296" formatCode="0.00"/>
     <numFmt numFmtId="297" formatCode="0.00"/>
-    <numFmt numFmtId="298" formatCode="0.0"/>
+    <numFmt numFmtId="298" formatCode="0.00"/>
     <numFmt numFmtId="299" formatCode="0.00"/>
     <numFmt numFmtId="300" formatCode="0.00"/>
-    <numFmt numFmtId="301" formatCode="0.00"/>
+    <numFmt numFmtId="301" formatCode="0.0"/>
     <numFmt numFmtId="302" formatCode="0.00"/>
     <numFmt numFmtId="303" formatCode="0.00"/>
     <numFmt numFmtId="304" formatCode="0.00"/>
@@ -2439,6 +2439,16 @@
     <numFmt numFmtId="361" formatCode="0.00"/>
     <numFmt numFmtId="362" formatCode="0.00"/>
     <numFmt numFmtId="363" formatCode="0.00"/>
+    <numFmt numFmtId="364" formatCode="0.00"/>
+    <numFmt numFmtId="365" formatCode="0.00"/>
+    <numFmt numFmtId="366" formatCode="0.00"/>
+    <numFmt numFmtId="367" formatCode="0.00"/>
+    <numFmt numFmtId="368" formatCode="0.00"/>
+    <numFmt numFmtId="369" formatCode="0.00"/>
+    <numFmt numFmtId="370" formatCode="0.00"/>
+    <numFmt numFmtId="371" formatCode="0.00"/>
+    <numFmt numFmtId="372" formatCode="0.00"/>
+    <numFmt numFmtId="373" formatCode="0.00"/>
   </numFmts>
   <fonts count="41">
     <font>
@@ -2935,7 +2945,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="387">
+  <cellXfs count="397">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3759,7 +3769,7 @@
     <xf numFmtId="273" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="274" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="274" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="275" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -3828,20 +3838,20 @@
     <xf numFmtId="296" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="297" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="297" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="298" fontId="31" fillId="16" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="298" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="299" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="300" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="301" fontId="31" fillId="16" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="299" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="300" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="301" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="302" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
@@ -3870,22 +3880,22 @@
     <xf numFmtId="310" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="311" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="311" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="312" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="312" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="313" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="313" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="314" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="314" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="315" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="315" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="316" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="316" fontId="38" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="317" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -4027,6 +4037,36 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="363" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="364" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="365" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="366" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="367" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="368" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="369" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="370" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="371" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="372" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="373" fontId="40" fillId="0" borderId="13" xfId="0" applyFont="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -13302,13 +13342,13 @@
         <v>167</v>
       </c>
       <c r="C15" s="198" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D15" s="200" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E15" s="202" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F15" s="204" t="s">
         <v>572</v>
@@ -13541,13 +13581,13 @@
         <v>408</v>
       </c>
       <c r="C20" s="214" t="n">
-        <v>9.53</v>
+        <v>9.22</v>
       </c>
       <c r="D20" s="216" t="n">
-        <v>9.53</v>
+        <v>9.22</v>
       </c>
       <c r="E20" s="218" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F20" s="204" t="s">
         <v>573</v>
@@ -13635,13 +13675,13 @@
         <v>182</v>
       </c>
       <c r="C22" s="215" t="n">
-        <v>49.01</v>
+        <v>50.5</v>
       </c>
       <c r="D22" s="217" t="n">
-        <v>49.01</v>
+        <v>50.5</v>
       </c>
       <c r="E22" s="219" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F22" s="205" t="s">
         <v>572</v>
@@ -14015,13 +14055,13 @@
         <v>197</v>
       </c>
       <c r="C30" s="244" t="n">
-        <v>3.81</v>
+        <v>3.36</v>
       </c>
       <c r="D30" s="246" t="str">
         <f>=IF(C30&lt;&gt;"",IF(C30&lt;18,round(C30/18*100,2),100),"")</f>
       </c>
       <c r="E30" s="248" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="F30" s="204" t="s">
         <v>573</v>
@@ -14246,16 +14286,26 @@
       <c r="B34" s="197" t="s">
         <v>206</v>
       </c>
-      <c r="C34" s="245"/>
+      <c r="C34" s="245" t="n">
+        <v>47</v>
+      </c>
       <c r="D34" s="247" t="str">
         <f/>
       </c>
-      <c r="E34" s="249"/>
-      <c r="F34" s="205"/>
+      <c r="E34" s="249" t="n">
+        <v>2020</v>
+      </c>
+      <c r="F34" s="205" t="s">
+        <v>573</v>
+      </c>
       <c r="G34" s="205"/>
       <c r="H34" s="95"/>
-      <c r="I34" s="251"/>
-      <c r="J34" s="253"/>
+      <c r="I34" s="251" t="n">
+        <v>35</v>
+      </c>
+      <c r="J34" s="253" t="n">
+        <v>61</v>
+      </c>
       <c r="K34" s="205"/>
       <c r="L34" s="255" t="str">
         <f/>
@@ -14268,8 +14318,12 @@
         <f>=IF(OR(ISBLANK(J34),ISBLANK(I34)),"",J34-I34)</f>
       </c>
       <c r="P34" s="205"/>
-      <c r="Q34" s="205"/>
-      <c r="R34" s="205"/>
+      <c r="Q34" s="205" t="s">
+        <v>573</v>
+      </c>
+      <c r="R34" s="205" t="s">
+        <v>574</v>
+      </c>
       <c r="S34" s="205"/>
       <c r="T34" s="205"/>
       <c r="U34" s="205"/>
@@ -16052,19 +16106,19 @@
       <c r="W6" s="287" t="n">
         <v>45.01</v>
       </c>
-      <c r="X6" s="296" t="n">
+      <c r="X6" s="297" t="n">
         <v>46.16</v>
       </c>
-      <c r="Y6" s="296" t="n">
+      <c r="Y6" s="297" t="n">
         <v>47.34</v>
       </c>
-      <c r="Z6" s="296" t="n">
+      <c r="Z6" s="297" t="n">
         <v>48.48</v>
       </c>
-      <c r="AA6" s="296" t="n">
+      <c r="AA6" s="297" t="n">
         <v>49.7</v>
       </c>
-      <c r="AB6" s="296" t="n">
+      <c r="AB6" s="297" t="n">
         <v>50.78</v>
       </c>
     </row>
@@ -16072,28 +16126,28 @@
       <c r="B7" s="287" t="s">
         <v>487</v>
       </c>
-      <c r="C7" s="313" t="n">
+      <c r="C7" s="315" t="n">
         <v>9.81</v>
       </c>
-      <c r="D7" s="313" t="n">
+      <c r="D7" s="315" t="n">
         <v>10.13</v>
       </c>
-      <c r="E7" s="313" t="n">
+      <c r="E7" s="315" t="n">
         <v>10.72</v>
       </c>
-      <c r="F7" s="313" t="n">
+      <c r="F7" s="315" t="n">
         <v>11.34</v>
       </c>
-      <c r="G7" s="313" t="n">
+      <c r="G7" s="315" t="n">
         <v>11.89</v>
       </c>
-      <c r="H7" s="313" t="n">
+      <c r="H7" s="315" t="n">
         <v>12.44</v>
       </c>
-      <c r="I7" s="313" t="n">
+      <c r="I7" s="315" t="n">
         <v>12.86</v>
       </c>
-      <c r="J7" s="313" t="n">
+      <c r="J7" s="315" t="n">
         <v>13.35</v>
       </c>
       <c r="K7" s="288" t="n">
@@ -16105,7 +16159,7 @@
       <c r="M7" s="288" t="n">
         <v>14.6</v>
       </c>
-      <c r="N7" s="313" t="n">
+      <c r="N7" s="315" t="n">
         <v>16.13</v>
       </c>
       <c r="O7" s="288" t="n">
@@ -16117,37 +16171,37 @@
       <c r="Q7" s="288" t="n">
         <v>16.3</v>
       </c>
-      <c r="R7" s="313" t="n">
+      <c r="R7" s="315" t="n">
         <v>19.03</v>
       </c>
-      <c r="S7" s="313" t="n">
+      <c r="S7" s="315" t="n">
         <v>19.67</v>
       </c>
       <c r="T7" s="288" t="n">
         <v>20.9</v>
       </c>
-      <c r="U7" s="297" t="n">
+      <c r="U7" s="298" t="n">
         <v>21.22</v>
       </c>
-      <c r="V7" s="297" t="n">
+      <c r="V7" s="298" t="n">
         <v>22.18</v>
       </c>
-      <c r="W7" s="297" t="n">
+      <c r="W7" s="298" t="n">
         <v>23.13</v>
       </c>
-      <c r="X7" s="297" t="n">
+      <c r="X7" s="298" t="n">
         <v>23.66</v>
       </c>
-      <c r="Y7" s="297" t="n">
+      <c r="Y7" s="298" t="n">
         <v>24.78</v>
       </c>
-      <c r="Z7" s="297" t="n">
+      <c r="Z7" s="298" t="n">
         <v>25.59</v>
       </c>
-      <c r="AA7" s="297" t="n">
+      <c r="AA7" s="298" t="n">
         <v>26.19</v>
       </c>
-      <c r="AB7" s="297" t="n">
+      <c r="AB7" s="298" t="n">
         <v>27.36</v>
       </c>
     </row>
@@ -16215,22 +16269,22 @@
       <c r="V8" s="287" t="n">
         <v>72</v>
       </c>
-      <c r="W8" s="298" t="n">
-        <v>70.09</v>
-      </c>
-      <c r="X8" s="298" t="n">
+      <c r="W8" s="287" t="n">
+        <v>70</v>
+      </c>
+      <c r="X8" s="299" t="n">
         <v>70.36</v>
       </c>
-      <c r="Y8" s="298" t="n">
+      <c r="Y8" s="299" t="n">
         <v>70.1</v>
       </c>
-      <c r="Z8" s="298" t="n">
+      <c r="Z8" s="299" t="n">
         <v>70.15</v>
       </c>
-      <c r="AA8" s="298" t="n">
+      <c r="AA8" s="299" t="n">
         <v>70.08</v>
       </c>
-      <c r="AB8" s="298" t="n">
+      <c r="AB8" s="299" t="n">
         <v>70.09</v>
       </c>
     </row>
@@ -16238,82 +16292,82 @@
       <c r="B9" s="287" t="s">
         <v>496</v>
       </c>
-      <c r="C9" s="314" t="n">
+      <c r="C9" s="316" t="n">
         <v>36.77</v>
       </c>
-      <c r="D9" s="314" t="n">
+      <c r="D9" s="316" t="n">
         <v>36.71</v>
       </c>
-      <c r="E9" s="314" t="n">
+      <c r="E9" s="316" t="n">
         <v>40.6</v>
       </c>
-      <c r="F9" s="314" t="n">
+      <c r="F9" s="316" t="n">
         <v>44.8</v>
       </c>
-      <c r="G9" s="314" t="n">
+      <c r="G9" s="316" t="n">
         <v>46.6</v>
       </c>
-      <c r="H9" s="314" t="n">
+      <c r="H9" s="316" t="n">
         <v>47.65</v>
       </c>
-      <c r="I9" s="314" t="n">
+      <c r="I9" s="316" t="n">
         <v>47.22</v>
       </c>
-      <c r="J9" s="314" t="n">
+      <c r="J9" s="316" t="n">
         <v>51.14</v>
       </c>
-      <c r="K9" s="314" t="n">
+      <c r="K9" s="316" t="n">
         <v>53.19</v>
       </c>
-      <c r="L9" s="314" t="n">
+      <c r="L9" s="316" t="n">
         <v>54.32</v>
       </c>
-      <c r="M9" s="314" t="n">
+      <c r="M9" s="316" t="n">
         <v>56.2</v>
       </c>
       <c r="N9" s="289" t="n">
         <v>60.5</v>
       </c>
-      <c r="O9" s="314" t="n">
+      <c r="O9" s="316" t="n">
         <v>59.58</v>
       </c>
-      <c r="P9" s="314" t="n">
+      <c r="P9" s="316" t="n">
         <v>61.77</v>
       </c>
-      <c r="Q9" s="314" t="n">
+      <c r="Q9" s="316" t="n">
         <v>63.22</v>
       </c>
       <c r="R9" s="289" t="n">
         <v>61.5</v>
       </c>
-      <c r="S9" s="314" t="n">
+      <c r="S9" s="316" t="n">
         <v>66.5</v>
       </c>
-      <c r="T9" s="314" t="n">
+      <c r="T9" s="316" t="n">
         <v>67.51</v>
       </c>
       <c r="U9" s="289" t="n">
         <v>67.7</v>
       </c>
-      <c r="V9" s="299" t="n">
+      <c r="V9" s="300" t="n">
         <v>69.51</v>
       </c>
-      <c r="W9" s="299" t="n">
+      <c r="W9" s="300" t="n">
         <v>71.52</v>
       </c>
-      <c r="X9" s="299" t="n">
+      <c r="X9" s="300" t="n">
         <v>72.9</v>
       </c>
-      <c r="Y9" s="299" t="n">
+      <c r="Y9" s="300" t="n">
         <v>73.14</v>
       </c>
-      <c r="Z9" s="299" t="n">
+      <c r="Z9" s="300" t="n">
         <v>74.48</v>
       </c>
-      <c r="AA9" s="299" t="n">
+      <c r="AA9" s="300" t="n">
         <v>75.68</v>
       </c>
-      <c r="AB9" s="299" t="n">
+      <c r="AB9" s="300" t="n">
         <v>76.52</v>
       </c>
     </row>
@@ -16384,19 +16438,19 @@
       <c r="W10" s="287" t="n">
         <v>61</v>
       </c>
-      <c r="X10" s="300" t="n">
+      <c r="X10" s="301" t="n">
         <v>61</v>
       </c>
-      <c r="Y10" s="300" t="n">
+      <c r="Y10" s="301" t="n">
         <v>61</v>
       </c>
-      <c r="Z10" s="300" t="n">
+      <c r="Z10" s="301" t="n">
         <v>61</v>
       </c>
-      <c r="AA10" s="300" t="n">
+      <c r="AA10" s="301" t="n">
         <v>61</v>
       </c>
-      <c r="AB10" s="300" t="n">
+      <c r="AB10" s="301" t="n">
         <v>61</v>
       </c>
     </row>
@@ -16464,22 +16518,22 @@
       <c r="V11" s="290" t="n">
         <v>9.53</v>
       </c>
-      <c r="W11" s="301" t="n">
-        <v>9.64</v>
-      </c>
-      <c r="X11" s="301" t="n">
+      <c r="W11" s="290" t="n">
+        <v>9.22</v>
+      </c>
+      <c r="X11" s="302" t="n">
         <v>10.57</v>
       </c>
-      <c r="Y11" s="301" t="n">
+      <c r="Y11" s="302" t="n">
         <v>10.82</v>
       </c>
-      <c r="Z11" s="301" t="n">
+      <c r="Z11" s="302" t="n">
         <v>11.47</v>
       </c>
-      <c r="AA11" s="301" t="n">
+      <c r="AA11" s="302" t="n">
         <v>12.02</v>
       </c>
-      <c r="AB11" s="301" t="n">
+      <c r="AB11" s="302" t="n">
         <v>12.62</v>
       </c>
     </row>
@@ -16578,22 +16632,22 @@
       <c r="V13" s="287" t="n">
         <v>49.01</v>
       </c>
-      <c r="W13" s="302" t="n">
-        <v>50.61</v>
-      </c>
-      <c r="X13" s="302" t="n">
+      <c r="W13" s="287" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="X13" s="303" t="n">
         <v>52.22</v>
       </c>
-      <c r="Y13" s="302" t="n">
+      <c r="Y13" s="303" t="n">
         <v>53.83</v>
       </c>
-      <c r="Z13" s="302" t="n">
+      <c r="Z13" s="303" t="n">
         <v>55.43</v>
       </c>
-      <c r="AA13" s="302" t="n">
+      <c r="AA13" s="303" t="n">
         <v>57.02</v>
       </c>
-      <c r="AB13" s="302" t="n">
+      <c r="AB13" s="303" t="n">
         <v>58.6</v>
       </c>
     </row>
@@ -16661,22 +16715,22 @@
       <c r="V14" s="287" t="n">
         <v>40.4</v>
       </c>
-      <c r="W14" s="303" t="n">
+      <c r="W14" s="304" t="n">
         <v>40.65</v>
       </c>
-      <c r="X14" s="303" t="n">
+      <c r="X14" s="304" t="n">
         <v>40.91</v>
       </c>
-      <c r="Y14" s="303" t="n">
+      <c r="Y14" s="304" t="n">
         <v>41.17</v>
       </c>
-      <c r="Z14" s="303" t="n">
+      <c r="Z14" s="304" t="n">
         <v>41.43</v>
       </c>
-      <c r="AA14" s="303" t="n">
+      <c r="AA14" s="304" t="n">
         <v>41.7</v>
       </c>
-      <c r="AB14" s="303" t="n">
+      <c r="AB14" s="304" t="n">
         <v>41.96</v>
       </c>
     </row>
@@ -16729,37 +16783,37 @@
       <c r="Q15" s="287" t="n">
         <v>5.37</v>
       </c>
-      <c r="R15" s="304" t="n">
+      <c r="R15" s="305" t="n">
         <v>5.39</v>
       </c>
-      <c r="S15" s="304" t="n">
+      <c r="S15" s="305" t="n">
         <v>5.42</v>
       </c>
-      <c r="T15" s="304" t="n">
+      <c r="T15" s="305" t="n">
         <v>5.44</v>
       </c>
-      <c r="U15" s="304" t="n">
+      <c r="U15" s="305" t="n">
         <v>5.47</v>
       </c>
-      <c r="V15" s="304" t="n">
+      <c r="V15" s="305" t="n">
         <v>5.49</v>
       </c>
-      <c r="W15" s="304" t="n">
+      <c r="W15" s="305" t="n">
         <v>5.52</v>
       </c>
-      <c r="X15" s="304" t="n">
+      <c r="X15" s="305" t="n">
         <v>5.54</v>
       </c>
-      <c r="Y15" s="304" t="n">
+      <c r="Y15" s="305" t="n">
         <v>5.57</v>
       </c>
-      <c r="Z15" s="304" t="n">
+      <c r="Z15" s="305" t="n">
         <v>5.59</v>
       </c>
-      <c r="AA15" s="304" t="n">
+      <c r="AA15" s="305" t="n">
         <v>5.62</v>
       </c>
-      <c r="AB15" s="304" t="n">
+      <c r="AB15" s="305" t="n">
         <v>5.65</v>
       </c>
     </row>
@@ -16770,55 +16824,55 @@
       <c r="C16" s="287" t="n">
         <v>36.85</v>
       </c>
-      <c r="D16" s="315" t="n">
+      <c r="D16" s="317" t="n">
         <v>36.01</v>
       </c>
-      <c r="E16" s="315" t="n">
+      <c r="E16" s="317" t="n">
         <v>35.17</v>
       </c>
-      <c r="F16" s="315" t="n">
+      <c r="F16" s="317" t="n">
         <v>34.33</v>
       </c>
-      <c r="G16" s="315" t="n">
+      <c r="G16" s="317" t="n">
         <v>33.49</v>
       </c>
       <c r="H16" s="287" t="n">
         <v>32.65</v>
       </c>
-      <c r="I16" s="315" t="n">
+      <c r="I16" s="317" t="n">
         <v>32</v>
       </c>
       <c r="J16" s="287" t="n">
         <v>31.35</v>
       </c>
-      <c r="K16" s="315" t="n">
+      <c r="K16" s="317" t="n">
         <v>30.6</v>
       </c>
-      <c r="L16" s="315" t="n">
+      <c r="L16" s="317" t="n">
         <v>29.85</v>
       </c>
       <c r="M16" s="287" t="n">
         <v>29.1</v>
       </c>
-      <c r="N16" s="315" t="n">
+      <c r="N16" s="317" t="n">
         <v>28.48</v>
       </c>
-      <c r="O16" s="315" t="n">
+      <c r="O16" s="317" t="n">
         <v>27.86</v>
       </c>
-      <c r="P16" s="315" t="n">
+      <c r="P16" s="317" t="n">
         <v>27.24</v>
       </c>
-      <c r="Q16" s="315" t="n">
+      <c r="Q16" s="317" t="n">
         <v>26.62</v>
       </c>
       <c r="R16" s="287" t="n">
         <v>26</v>
       </c>
-      <c r="S16" s="315" t="n">
+      <c r="S16" s="317" t="n">
         <v>25.45</v>
       </c>
-      <c r="T16" s="315" t="n">
+      <c r="T16" s="317" t="n">
         <v>24.9</v>
       </c>
       <c r="U16" s="287" t="n">
@@ -16827,22 +16881,22 @@
       <c r="V16" s="287" t="n">
         <v>23.8</v>
       </c>
-      <c r="W16" s="305" t="n">
+      <c r="W16" s="306" t="n">
         <v>23.3</v>
       </c>
-      <c r="X16" s="315" t="n">
+      <c r="X16" s="317" t="n">
         <v>22.8</v>
       </c>
-      <c r="Y16" s="315" t="n">
+      <c r="Y16" s="317" t="n">
         <v>22.3</v>
       </c>
-      <c r="Z16" s="305" t="n">
+      <c r="Z16" s="306" t="n">
         <v>21.8</v>
       </c>
-      <c r="AA16" s="315" t="n">
+      <c r="AA16" s="317" t="n">
         <v>21.4</v>
       </c>
-      <c r="AB16" s="305" t="n">
+      <c r="AB16" s="306" t="n">
         <v>21</v>
       </c>
     </row>
@@ -16910,22 +16964,22 @@
       <c r="V17" s="291" t="n">
         <v>3.81</v>
       </c>
-      <c r="W17" s="306" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="X17" s="306" t="n">
+      <c r="W17" s="291" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="X17" s="307" t="n">
         <v>3.52</v>
       </c>
-      <c r="Y17" s="306" t="n">
+      <c r="Y17" s="307" t="n">
         <v>3.37</v>
       </c>
-      <c r="Z17" s="306" t="n">
+      <c r="Z17" s="307" t="n">
         <v>3.23</v>
       </c>
-      <c r="AA17" s="306" t="n">
+      <c r="AA17" s="307" t="n">
         <v>3.1</v>
       </c>
-      <c r="AB17" s="306" t="n">
+      <c r="AB17" s="307" t="n">
         <v>2.97</v>
       </c>
     </row>
@@ -16933,22 +16987,22 @@
       <c r="B18" s="287" t="s">
         <v>535</v>
       </c>
-      <c r="C18" s="316" t="n">
+      <c r="C18" s="318" t="n">
         <v>7.72</v>
       </c>
-      <c r="D18" s="316" t="n">
+      <c r="D18" s="318" t="n">
         <v>7.72</v>
       </c>
-      <c r="E18" s="316" t="n">
+      <c r="E18" s="318" t="n">
         <v>7.66</v>
       </c>
-      <c r="F18" s="316" t="n">
+      <c r="F18" s="318" t="n">
         <v>7.6</v>
       </c>
-      <c r="G18" s="316" t="n">
+      <c r="G18" s="318" t="n">
         <v>7.54</v>
       </c>
-      <c r="H18" s="316" t="n">
+      <c r="H18" s="318" t="n">
         <v>7.48</v>
       </c>
       <c r="I18" s="292" t="n">
@@ -16963,13 +17017,13 @@
       <c r="L18" s="292" t="n">
         <v>8.2</v>
       </c>
-      <c r="M18" s="316" t="n">
+      <c r="M18" s="318" t="n">
         <v>7.55</v>
       </c>
-      <c r="N18" s="316" t="n">
+      <c r="N18" s="318" t="n">
         <v>6.8</v>
       </c>
-      <c r="O18" s="316" t="n">
+      <c r="O18" s="318" t="n">
         <v>5.8</v>
       </c>
       <c r="P18" s="292" t="n">
@@ -16984,31 +17038,31 @@
       <c r="S18" s="292" t="n">
         <v>4.26</v>
       </c>
-      <c r="T18" s="316" t="n">
+      <c r="T18" s="318" t="n">
         <v>4.54</v>
       </c>
-      <c r="U18" s="307" t="n">
+      <c r="U18" s="308" t="n">
         <v>7.24</v>
       </c>
-      <c r="V18" s="307" t="n">
+      <c r="V18" s="308" t="n">
         <v>7.24</v>
       </c>
-      <c r="W18" s="307" t="n">
+      <c r="W18" s="308" t="n">
         <v>7.24</v>
       </c>
-      <c r="X18" s="307" t="n">
+      <c r="X18" s="308" t="n">
         <v>7.97</v>
       </c>
-      <c r="Y18" s="307" t="n">
+      <c r="Y18" s="308" t="n">
         <v>8.7</v>
       </c>
-      <c r="Z18" s="307" t="n">
+      <c r="Z18" s="308" t="n">
         <v>9.43</v>
       </c>
-      <c r="AA18" s="307" t="n">
+      <c r="AA18" s="308" t="n">
         <v>10.16</v>
       </c>
-      <c r="AB18" s="307" t="n">
+      <c r="AB18" s="308" t="n">
         <v>10.89</v>
       </c>
     </row>
@@ -17016,22 +17070,22 @@
       <c r="B19" s="287" t="s">
         <v>539</v>
       </c>
-      <c r="C19" s="317" t="n">
+      <c r="C19" s="319" t="n">
         <v>1.9</v>
       </c>
       <c r="D19" s="293" t="n">
         <v>1.9</v>
       </c>
-      <c r="E19" s="317" t="n">
+      <c r="E19" s="319" t="n">
         <v>1.84</v>
       </c>
-      <c r="F19" s="317" t="n">
+      <c r="F19" s="319" t="n">
         <v>1.78</v>
       </c>
-      <c r="G19" s="317" t="n">
+      <c r="G19" s="319" t="n">
         <v>1.72</v>
       </c>
-      <c r="H19" s="317" t="n">
+      <c r="H19" s="319" t="n">
         <v>1.66</v>
       </c>
       <c r="I19" s="293" t="n">
@@ -17067,31 +17121,31 @@
       <c r="S19" s="293" t="n">
         <v>2.78</v>
       </c>
-      <c r="T19" s="317" t="n">
+      <c r="T19" s="319" t="n">
         <v>2.78</v>
       </c>
-      <c r="U19" s="308" t="n">
+      <c r="U19" s="309" t="n">
         <v>2.78</v>
       </c>
-      <c r="V19" s="308" t="n">
+      <c r="V19" s="309" t="n">
         <v>2.78</v>
       </c>
-      <c r="W19" s="308" t="n">
+      <c r="W19" s="309" t="n">
         <v>2.78</v>
       </c>
-      <c r="X19" s="308" t="n">
+      <c r="X19" s="309" t="n">
         <v>2.83</v>
       </c>
-      <c r="Y19" s="308" t="n">
+      <c r="Y19" s="309" t="n">
         <v>2.87</v>
       </c>
-      <c r="Z19" s="308" t="n">
+      <c r="Z19" s="309" t="n">
         <v>2.91</v>
       </c>
-      <c r="AA19" s="308" t="n">
+      <c r="AA19" s="309" t="n">
         <v>2.96</v>
       </c>
-      <c r="AB19" s="308" t="n">
+      <c r="AB19" s="309" t="n">
         <v>3</v>
       </c>
     </row>
@@ -17099,19 +17153,19 @@
       <c r="B20" s="287" t="s">
         <v>543</v>
       </c>
-      <c r="C20" s="318" t="n">
+      <c r="C20" s="320" t="n">
         <v>5.82</v>
       </c>
-      <c r="D20" s="318" t="n">
+      <c r="D20" s="320" t="n">
         <v>5.82</v>
       </c>
-      <c r="E20" s="318" t="n">
+      <c r="E20" s="320" t="n">
         <v>5.82</v>
       </c>
-      <c r="F20" s="318" t="n">
+      <c r="F20" s="320" t="n">
         <v>5.82</v>
       </c>
-      <c r="G20" s="318" t="n">
+      <c r="G20" s="320" t="n">
         <v>5.82</v>
       </c>
       <c r="H20" s="294" t="n">
@@ -17129,13 +17183,13 @@
       <c r="L20" s="294" t="n">
         <v>6.08</v>
       </c>
-      <c r="M20" s="318" t="n">
+      <c r="M20" s="320" t="n">
         <v>5.18</v>
       </c>
-      <c r="N20" s="318" t="n">
+      <c r="N20" s="320" t="n">
         <v>4.29</v>
       </c>
-      <c r="O20" s="318" t="n">
+      <c r="O20" s="320" t="n">
         <v>3.39</v>
       </c>
       <c r="P20" s="294" t="n">
@@ -17156,25 +17210,25 @@
       <c r="U20" s="294" t="n">
         <v>4.46</v>
       </c>
-      <c r="V20" s="309" t="n">
+      <c r="V20" s="310" t="n">
         <v>4.46</v>
       </c>
-      <c r="W20" s="309" t="n">
+      <c r="W20" s="310" t="n">
         <v>4.46</v>
       </c>
-      <c r="X20" s="309" t="n">
+      <c r="X20" s="310" t="n">
         <v>5.14</v>
       </c>
-      <c r="Y20" s="309" t="n">
+      <c r="Y20" s="310" t="n">
         <v>5.83</v>
       </c>
-      <c r="Z20" s="309" t="n">
+      <c r="Z20" s="310" t="n">
         <v>6.52</v>
       </c>
-      <c r="AA20" s="309" t="n">
+      <c r="AA20" s="310" t="n">
         <v>7.2</v>
       </c>
-      <c r="AB20" s="309" t="n">
+      <c r="AB20" s="310" t="n">
         <v>7.89</v>
       </c>
     </row>
@@ -17182,110 +17236,214 @@
       <c r="B21" s="287" t="s">
         <v>547</v>
       </c>
-      <c r="C21" s="287"/>
-      <c r="D21" s="287"/>
-      <c r="E21" s="287"/>
-      <c r="F21" s="287"/>
-      <c r="G21" s="287"/>
-      <c r="H21" s="287"/>
-      <c r="I21" s="287"/>
-      <c r="J21" s="287"/>
-      <c r="K21" s="287"/>
-      <c r="L21" s="287"/>
-      <c r="M21" s="287"/>
-      <c r="N21" s="287"/>
-      <c r="O21" s="287"/>
-      <c r="P21" s="287"/>
-      <c r="Q21" s="287"/>
-      <c r="R21" s="287"/>
-      <c r="S21" s="287"/>
-      <c r="T21" s="287"/>
-      <c r="U21" s="287"/>
-      <c r="V21" s="287"/>
-      <c r="W21" s="287"/>
-      <c r="X21" s="287"/>
-      <c r="Y21" s="287"/>
-      <c r="Z21" s="287"/>
-      <c r="AA21" s="287"/>
-      <c r="AB21" s="287"/>
+      <c r="C21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="D21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="E21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="F21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="G21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="H21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="I21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="J21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="K21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="L21" s="321" t="n">
+        <v>45</v>
+      </c>
+      <c r="M21" s="295" t="n">
+        <v>45</v>
+      </c>
+      <c r="N21" s="295" t="n">
+        <v>25</v>
+      </c>
+      <c r="O21" s="295" t="n">
+        <v>25</v>
+      </c>
+      <c r="P21" s="295" t="n">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="295" t="n">
+        <v>46</v>
+      </c>
+      <c r="R21" s="295" t="n">
+        <v>43</v>
+      </c>
+      <c r="S21" s="295" t="n">
+        <v>42</v>
+      </c>
+      <c r="T21" s="295" t="n">
+        <v>41.78</v>
+      </c>
+      <c r="U21" s="295" t="n">
+        <v>35</v>
+      </c>
+      <c r="V21" s="295" t="n">
+        <v>43</v>
+      </c>
+      <c r="W21" s="295" t="n">
+        <v>47</v>
+      </c>
+      <c r="X21" s="311" t="n">
+        <v>49</v>
+      </c>
+      <c r="Y21" s="311" t="n">
+        <v>52</v>
+      </c>
+      <c r="Z21" s="311" t="n">
+        <v>55</v>
+      </c>
+      <c r="AA21" s="311" t="n">
+        <v>58</v>
+      </c>
+      <c r="AB21" s="311" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="22" ht="15" customHeight="1">
       <c r="B22" s="287" t="s">
         <v>551</v>
       </c>
-      <c r="C22" s="319"/>
-      <c r="D22" s="319"/>
-      <c r="E22" s="319"/>
-      <c r="F22" s="319"/>
-      <c r="G22" s="319"/>
-      <c r="H22" s="319"/>
-      <c r="I22" s="319"/>
-      <c r="J22" s="295" t="n">
+      <c r="C22" s="322"/>
+      <c r="D22" s="322"/>
+      <c r="E22" s="322"/>
+      <c r="F22" s="322"/>
+      <c r="G22" s="322"/>
+      <c r="H22" s="322"/>
+      <c r="I22" s="322"/>
+      <c r="J22" s="296" t="n">
         <v>4.84</v>
       </c>
-      <c r="K22" s="319"/>
-      <c r="L22" s="319"/>
+      <c r="K22" s="322"/>
+      <c r="L22" s="322"/>
       <c r="M22" s="287" t="n">
         <v>9.73</v>
       </c>
-      <c r="N22" s="319"/>
-      <c r="O22" s="319"/>
-      <c r="P22" s="295" t="n">
+      <c r="N22" s="322"/>
+      <c r="O22" s="322"/>
+      <c r="P22" s="296" t="n">
         <v>14.63</v>
       </c>
-      <c r="Q22" s="319"/>
+      <c r="Q22" s="322"/>
       <c r="R22" s="287" t="n">
         <v>16.84</v>
       </c>
-      <c r="S22" s="295" t="n">
+      <c r="S22" s="296" t="n">
         <v>23.84</v>
       </c>
       <c r="T22" s="287" t="n">
         <v>24.35</v>
       </c>
-      <c r="U22" s="310"/>
-      <c r="V22" s="310"/>
-      <c r="W22" s="310"/>
-      <c r="X22" s="310"/>
-      <c r="Y22" s="310"/>
-      <c r="Z22" s="310"/>
-      <c r="AA22" s="310"/>
-      <c r="AB22" s="310"/>
+      <c r="U22" s="312"/>
+      <c r="V22" s="312"/>
+      <c r="W22" s="312"/>
+      <c r="X22" s="312"/>
+      <c r="Y22" s="312"/>
+      <c r="Z22" s="312"/>
+      <c r="AA22" s="312"/>
+      <c r="AB22" s="312"/>
     </row>
     <row r="23">
       <c r="B23" s="284" t="s">
         <v>624</v>
       </c>
-      <c r="C23" s="287"/>
-      <c r="D23" s="287"/>
-      <c r="E23" s="287"/>
-      <c r="F23" s="287"/>
-      <c r="G23" s="287"/>
-      <c r="H23" s="287"/>
-      <c r="I23" s="287"/>
-      <c r="J23" s="287"/>
-      <c r="K23" s="287"/>
-      <c r="L23" s="287"/>
-      <c r="M23" s="287"/>
-      <c r="N23" s="287"/>
-      <c r="O23" s="287"/>
-      <c r="P23" s="287"/>
-      <c r="Q23" s="287"/>
-      <c r="R23" s="287"/>
-      <c r="S23" s="287"/>
-      <c r="T23" s="287"/>
-      <c r="U23" s="287"/>
-      <c r="V23" s="287"/>
-      <c r="W23" s="311"/>
-      <c r="X23" s="311"/>
-      <c r="Y23" s="311"/>
-      <c r="Z23" s="311"/>
-      <c r="AA23" s="311"/>
-      <c r="AB23" s="311"/>
+      <c r="C23" s="287" t="n">
+        <v>30.47</v>
+      </c>
+      <c r="D23" s="287" t="n">
+        <v>32.2</v>
+      </c>
+      <c r="E23" s="287" t="n">
+        <v>33.52</v>
+      </c>
+      <c r="F23" s="287" t="n">
+        <v>34.34</v>
+      </c>
+      <c r="G23" s="287" t="n">
+        <v>35.99</v>
+      </c>
+      <c r="H23" s="287" t="n">
+        <v>37.44</v>
+      </c>
+      <c r="I23" s="287" t="n">
+        <v>38.03</v>
+      </c>
+      <c r="J23" s="287" t="n">
+        <v>39.2</v>
+      </c>
+      <c r="K23" s="287" t="n">
+        <v>39.52</v>
+      </c>
+      <c r="L23" s="287" t="n">
+        <v>38.92</v>
+      </c>
+      <c r="M23" s="287" t="n">
+        <v>39.84</v>
+      </c>
+      <c r="N23" s="287" t="n">
+        <v>38.59</v>
+      </c>
+      <c r="O23" s="287" t="n">
+        <v>39</v>
+      </c>
+      <c r="P23" s="287" t="n">
+        <v>39.76</v>
+      </c>
+      <c r="Q23" s="287" t="n">
+        <v>40.61</v>
+      </c>
+      <c r="R23" s="287" t="n">
+        <v>41.09</v>
+      </c>
+      <c r="S23" s="287" t="n">
+        <v>42.47</v>
+      </c>
+      <c r="T23" s="287" t="n">
+        <v>43.23</v>
+      </c>
+      <c r="U23" s="287" t="n">
+        <v>43.3</v>
+      </c>
+      <c r="V23" s="287" t="n">
+        <v>44.54</v>
+      </c>
+      <c r="W23" s="287" t="n">
+        <v>43.79</v>
+      </c>
+      <c r="X23" s="287" t="n">
+        <v>44.45</v>
+      </c>
+      <c r="Y23" s="313" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="Z23" s="313" t="n">
+        <v>45.4</v>
+      </c>
+      <c r="AA23" s="313" t="n">
+        <v>45.89</v>
+      </c>
+      <c r="AB23" s="313" t="n">
+        <v>46.39</v>
+      </c>
     </row>
     <row r="24">
-      <c r="B24" s="285" t="s">
-        <v>625</v>
+      <c r="B24" s="284" t="s">
+        <v>575</v>
       </c>
       <c r="C24" s="287"/>
       <c r="D24" s="287"/>
@@ -17294,29 +17452,57 @@
       <c r="G24" s="287"/>
       <c r="H24" s="287"/>
       <c r="I24" s="287"/>
-      <c r="J24" s="287"/>
+      <c r="J24" s="287" t="n">
+        <v>37.31</v>
+      </c>
       <c r="K24" s="287"/>
       <c r="L24" s="287"/>
-      <c r="M24" s="287"/>
+      <c r="M24" s="287" t="n">
+        <v>35.96</v>
+      </c>
       <c r="N24" s="287"/>
       <c r="O24" s="287"/>
-      <c r="P24" s="287"/>
+      <c r="P24" s="287" t="n">
+        <v>33.94</v>
+      </c>
       <c r="Q24" s="287"/>
-      <c r="R24" s="287"/>
-      <c r="S24" s="287"/>
-      <c r="T24" s="287"/>
-      <c r="U24" s="287"/>
-      <c r="V24" s="287"/>
-      <c r="W24" s="312"/>
-      <c r="X24" s="312"/>
-      <c r="Y24" s="312"/>
-      <c r="Z24" s="312"/>
-      <c r="AA24" s="312"/>
-      <c r="AB24" s="312"/>
+      <c r="R24" s="287" t="n">
+        <v>34.17</v>
+      </c>
+      <c r="S24" s="287" t="n">
+        <v>32.35</v>
+      </c>
+      <c r="T24" s="287" t="n">
+        <v>32.7</v>
+      </c>
+      <c r="U24" s="287" t="n">
+        <v>31.73</v>
+      </c>
+      <c r="V24" s="287" t="n">
+        <v>31.59</v>
+      </c>
+      <c r="W24" s="287" t="n">
+        <v>30.04</v>
+      </c>
+      <c r="X24" s="287" t="n">
+        <v>29.44</v>
+      </c>
+      <c r="Y24" s="314" t="n">
+        <v>28.67</v>
+      </c>
+      <c r="Z24" s="314" t="n">
+        <v>27.94</v>
+      </c>
+      <c r="AA24" s="314" t="n">
+        <v>27.16</v>
+      </c>
+      <c r="AB24" s="314" t="n">
+        <v>26.36</v>
+      </c>
     </row>
     <row r="25">
-      <c r="B25" s="149" t="s">
-        <v>149</v>
+      <c r="B25" s="285" t="s">
+        <v>625</v>
       </c>
       <c r="C25" s="149"/>
       <c r="D25" s="149"/>
@@ -17515,28 +17701,28 @@
       <c r="C6" s="284" t="s">
         <v>483</v>
       </c>
-      <c r="D6" s="320" t="n">
+      <c r="D6" s="323" t="n">
         <v>42.97</v>
       </c>
-      <c r="E6" s="320" t="n">
+      <c r="E6" s="323" t="n">
         <v>43.92</v>
       </c>
-      <c r="F6" s="320" t="n">
+      <c r="F6" s="323" t="n">
         <v>45.01</v>
       </c>
-      <c r="G6" s="320" t="n">
+      <c r="G6" s="323" t="n">
         <v>46.16</v>
       </c>
-      <c r="H6" s="320" t="n">
+      <c r="H6" s="323" t="n">
         <v>47.34</v>
       </c>
-      <c r="I6" s="320" t="n">
+      <c r="I6" s="323" t="n">
         <v>48.48</v>
       </c>
-      <c r="J6" s="320" t="n">
+      <c r="J6" s="323" t="n">
         <v>49.7</v>
       </c>
-      <c r="K6" s="320" t="n">
+      <c r="K6" s="323" t="n">
         <v>50.78</v>
       </c>
       <c r="L6" s="186"/>
@@ -17551,35 +17737,35 @@
     </row>
     <row r="7" outlineLevel="1" hidden="0">
       <c r="A7" s="186"/>
-      <c r="B7" s="320" t="s">
+      <c r="B7" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C7" s="320" t="s">
+      <c r="C7" s="323" t="s">
         <v>483</v>
       </c>
-      <c r="D7" s="320" t="n">
+      <c r="D7" s="323" t="n">
         <v>42.97</v>
       </c>
-      <c r="E7" s="320" t="n">
+      <c r="E7" s="323" t="n">
         <v>43.92</v>
       </c>
-      <c r="F7" s="320" t="n">
+      <c r="F7" s="323" t="n">
         <v>45.01</v>
       </c>
-      <c r="G7" s="333" t="n">
-        <v>46.16</v>
-      </c>
-      <c r="H7" s="333" t="n">
-        <v>47.34</v>
-      </c>
-      <c r="I7" s="333" t="n">
-        <v>48.48</v>
-      </c>
-      <c r="J7" s="333" t="n">
-        <v>49.7</v>
-      </c>
-      <c r="K7" s="333" t="n">
-        <v>50.78</v>
+      <c r="G7" s="339" t="n">
+        <v>45.01</v>
+      </c>
+      <c r="H7" s="339" t="n">
+        <v>46.15</v>
+      </c>
+      <c r="I7" s="339" t="n">
+        <v>47.3</v>
+      </c>
+      <c r="J7" s="339" t="n">
+        <v>48.44</v>
+      </c>
+      <c r="K7" s="339" t="n">
+        <v>49.58</v>
       </c>
       <c r="L7" s="186"/>
       <c r="M7" s="186"/>
@@ -17593,35 +17779,35 @@
     </row>
     <row r="8" outlineLevel="1" hidden="0">
       <c r="A8" s="186"/>
-      <c r="B8" s="320" t="s">
+      <c r="B8" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C8" s="320" t="s">
+      <c r="C8" s="323" t="s">
         <v>483</v>
       </c>
-      <c r="D8" s="320" t="n">
+      <c r="D8" s="323" t="n">
         <v>42.97</v>
       </c>
-      <c r="E8" s="320" t="n">
-        <v>42.97</v>
-      </c>
-      <c r="F8" s="320" t="n">
-        <v>42.97</v>
-      </c>
-      <c r="G8" s="334" t="n">
-        <v>42.97</v>
-      </c>
-      <c r="H8" s="334" t="n">
-        <v>42.97</v>
-      </c>
-      <c r="I8" s="334" t="n">
-        <v>42.97</v>
-      </c>
-      <c r="J8" s="334" t="n">
-        <v>42.97</v>
-      </c>
-      <c r="K8" s="334" t="n">
-        <v>42.97</v>
+      <c r="E8" s="323" t="n">
+        <v>43.92</v>
+      </c>
+      <c r="F8" s="323" t="n">
+        <v>45.01</v>
+      </c>
+      <c r="G8" s="340" t="n">
+        <v>46.16</v>
+      </c>
+      <c r="H8" s="340" t="n">
+        <v>47.34</v>
+      </c>
+      <c r="I8" s="340" t="n">
+        <v>48.48</v>
+      </c>
+      <c r="J8" s="340" t="n">
+        <v>49.7</v>
+      </c>
+      <c r="K8" s="340" t="n">
+        <v>50.78</v>
       </c>
       <c r="L8" s="186"/>
       <c r="M8" s="186"/>
@@ -17641,28 +17827,28 @@
       <c r="C9" s="284" t="s">
         <v>487</v>
       </c>
-      <c r="D9" s="320" t="n">
+      <c r="D9" s="323" t="n">
         <v>21.22</v>
       </c>
-      <c r="E9" s="320" t="n">
+      <c r="E9" s="323" t="n">
         <v>22.18</v>
       </c>
-      <c r="F9" s="320" t="n">
+      <c r="F9" s="323" t="n">
         <v>23.13</v>
       </c>
-      <c r="G9" s="335" t="n">
+      <c r="G9" s="341" t="n">
         <v>23.66</v>
       </c>
-      <c r="H9" s="335" t="n">
+      <c r="H9" s="341" t="n">
         <v>24.78</v>
       </c>
-      <c r="I9" s="335" t="n">
+      <c r="I9" s="341" t="n">
         <v>25.59</v>
       </c>
-      <c r="J9" s="335" t="n">
+      <c r="J9" s="341" t="n">
         <v>26.19</v>
       </c>
-      <c r="K9" s="335" t="n">
+      <c r="K9" s="341" t="n">
         <v>27.36</v>
       </c>
       <c r="L9" s="186"/>
@@ -17677,35 +17863,35 @@
     </row>
     <row r="10" outlineLevel="1" hidden="0">
       <c r="A10" s="186"/>
-      <c r="B10" s="320" t="s">
+      <c r="B10" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C10" s="320" t="s">
+      <c r="C10" s="323" t="s">
         <v>487</v>
       </c>
-      <c r="D10" s="336" t="n">
+      <c r="D10" s="342" t="n">
         <v>21.22</v>
       </c>
-      <c r="E10" s="336" t="n">
-        <v>23.82</v>
-      </c>
-      <c r="F10" s="336" t="n">
-        <v>26.42</v>
-      </c>
-      <c r="G10" s="336" t="n">
-        <v>29.02</v>
-      </c>
-      <c r="H10" s="336" t="n">
-        <v>31.62</v>
-      </c>
-      <c r="I10" s="336" t="n">
-        <v>34.22</v>
-      </c>
-      <c r="J10" s="336" t="n">
-        <v>36.82</v>
-      </c>
-      <c r="K10" s="336" t="n">
-        <v>39.42</v>
+      <c r="E10" s="342" t="n">
+        <v>22.18</v>
+      </c>
+      <c r="F10" s="342" t="n">
+        <v>23.13</v>
+      </c>
+      <c r="G10" s="342" t="n">
+        <v>23.66</v>
+      </c>
+      <c r="H10" s="342" t="n">
+        <v>24.78</v>
+      </c>
+      <c r="I10" s="342" t="n">
+        <v>25.59</v>
+      </c>
+      <c r="J10" s="342" t="n">
+        <v>26.19</v>
+      </c>
+      <c r="K10" s="342" t="n">
+        <v>27.36</v>
       </c>
       <c r="L10" s="186"/>
       <c r="M10" s="186"/>
@@ -17719,35 +17905,35 @@
     </row>
     <row r="11" outlineLevel="1" hidden="0">
       <c r="A11" s="186"/>
-      <c r="B11" s="320" t="s">
+      <c r="B11" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C11" s="320" t="s">
+      <c r="C11" s="323" t="s">
         <v>487</v>
       </c>
-      <c r="D11" s="337" t="n">
+      <c r="D11" s="343" t="n">
         <v>21.22</v>
       </c>
-      <c r="E11" s="337" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="F11" s="337" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="G11" s="337" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="H11" s="337" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="I11" s="337" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="J11" s="337" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="K11" s="337" t="n">
-        <v>21.22</v>
+      <c r="E11" s="343" t="n">
+        <v>22.18</v>
+      </c>
+      <c r="F11" s="343" t="n">
+        <v>23.13</v>
+      </c>
+      <c r="G11" s="343" t="n">
+        <v>23.66</v>
+      </c>
+      <c r="H11" s="343" t="n">
+        <v>24.78</v>
+      </c>
+      <c r="I11" s="343" t="n">
+        <v>25.59</v>
+      </c>
+      <c r="J11" s="343" t="n">
+        <v>26.19</v>
+      </c>
+      <c r="K11" s="343" t="n">
+        <v>27.36</v>
       </c>
       <c r="L11" s="186"/>
       <c r="M11" s="186"/>
@@ -17767,28 +17953,28 @@
       <c r="C12" s="284" t="s">
         <v>492</v>
       </c>
-      <c r="D12" s="338" t="n">
+      <c r="D12" s="344" t="n">
         <v>72</v>
       </c>
-      <c r="E12" s="338" t="n">
+      <c r="E12" s="344" t="n">
         <v>72</v>
       </c>
-      <c r="F12" s="338" t="n">
-        <v>70.09</v>
-      </c>
-      <c r="G12" s="338" t="n">
+      <c r="F12" s="344" t="n">
+        <v>70</v>
+      </c>
+      <c r="G12" s="344" t="n">
         <v>70.36</v>
       </c>
-      <c r="H12" s="338" t="n">
+      <c r="H12" s="344" t="n">
         <v>70.1</v>
       </c>
-      <c r="I12" s="338" t="n">
+      <c r="I12" s="344" t="n">
         <v>70.15</v>
       </c>
-      <c r="J12" s="338" t="n">
+      <c r="J12" s="344" t="n">
         <v>70.08</v>
       </c>
-      <c r="K12" s="338" t="n">
+      <c r="K12" s="344" t="n">
         <v>70.09</v>
       </c>
       <c r="L12" s="186"/>
@@ -17803,35 +17989,35 @@
     </row>
     <row r="13" outlineLevel="1" hidden="0">
       <c r="A13" s="186"/>
-      <c r="B13" s="320" t="s">
+      <c r="B13" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C13" s="320" t="s">
+      <c r="C13" s="323" t="s">
         <v>492</v>
       </c>
-      <c r="D13" s="320" t="n">
+      <c r="D13" s="323" t="n">
         <v>72</v>
       </c>
-      <c r="E13" s="320" t="n">
+      <c r="E13" s="323" t="n">
         <v>72</v>
       </c>
-      <c r="F13" s="339" t="n">
-        <v>72</v>
-      </c>
-      <c r="G13" s="339" t="n">
-        <v>73.06</v>
-      </c>
-      <c r="H13" s="339" t="n">
-        <v>74.11</v>
-      </c>
-      <c r="I13" s="339" t="n">
-        <v>75.17</v>
-      </c>
-      <c r="J13" s="339" t="n">
-        <v>76.22</v>
-      </c>
-      <c r="K13" s="339" t="n">
-        <v>77.28</v>
+      <c r="F13" s="323" t="n">
+        <v>70</v>
+      </c>
+      <c r="G13" s="345" t="n">
+        <v>70</v>
+      </c>
+      <c r="H13" s="345" t="n">
+        <v>69.68</v>
+      </c>
+      <c r="I13" s="345" t="n">
+        <v>69.36</v>
+      </c>
+      <c r="J13" s="345" t="n">
+        <v>69.05</v>
+      </c>
+      <c r="K13" s="345" t="n">
+        <v>68.73</v>
       </c>
       <c r="L13" s="186"/>
       <c r="M13" s="186"/>
@@ -17845,35 +18031,35 @@
     </row>
     <row r="14" outlineLevel="1" hidden="0">
       <c r="A14" s="186"/>
-      <c r="B14" s="320" t="s">
+      <c r="B14" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C14" s="320" t="s">
+      <c r="C14" s="323" t="s">
         <v>492</v>
       </c>
-      <c r="D14" s="320" t="n">
+      <c r="D14" s="323" t="n">
         <v>72</v>
       </c>
-      <c r="E14" s="320" t="n">
+      <c r="E14" s="323" t="n">
         <v>72</v>
       </c>
-      <c r="F14" s="340" t="n">
-        <v>72</v>
-      </c>
-      <c r="G14" s="340" t="n">
-        <v>72</v>
-      </c>
-      <c r="H14" s="340" t="n">
-        <v>72</v>
-      </c>
-      <c r="I14" s="340" t="n">
-        <v>72</v>
-      </c>
-      <c r="J14" s="340" t="n">
-        <v>72</v>
-      </c>
-      <c r="K14" s="340" t="n">
-        <v>72</v>
+      <c r="F14" s="323" t="n">
+        <v>70</v>
+      </c>
+      <c r="G14" s="346" t="n">
+        <v>70.36</v>
+      </c>
+      <c r="H14" s="346" t="n">
+        <v>70.1</v>
+      </c>
+      <c r="I14" s="346" t="n">
+        <v>70.15</v>
+      </c>
+      <c r="J14" s="346" t="n">
+        <v>70.08</v>
+      </c>
+      <c r="K14" s="346" t="n">
+        <v>70.09</v>
       </c>
       <c r="L14" s="186"/>
       <c r="M14" s="186"/>
@@ -17893,28 +18079,28 @@
       <c r="C15" s="284" t="s">
         <v>496</v>
       </c>
-      <c r="D15" s="320" t="n">
+      <c r="D15" s="323" t="n">
         <v>67.7</v>
       </c>
-      <c r="E15" s="320" t="n">
+      <c r="E15" s="323" t="n">
         <v>69.51</v>
       </c>
-      <c r="F15" s="341" t="n">
+      <c r="F15" s="323" t="n">
         <v>71.52</v>
       </c>
-      <c r="G15" s="341" t="n">
+      <c r="G15" s="347" t="n">
         <v>72.9</v>
       </c>
-      <c r="H15" s="341" t="n">
+      <c r="H15" s="347" t="n">
         <v>73.14</v>
       </c>
-      <c r="I15" s="341" t="n">
+      <c r="I15" s="347" t="n">
         <v>74.48</v>
       </c>
-      <c r="J15" s="341" t="n">
+      <c r="J15" s="347" t="n">
         <v>75.68</v>
       </c>
-      <c r="K15" s="341" t="n">
+      <c r="K15" s="347" t="n">
         <v>76.52</v>
       </c>
       <c r="L15" s="186"/>
@@ -17929,35 +18115,35 @@
     </row>
     <row r="16" outlineLevel="1" hidden="0">
       <c r="A16" s="186"/>
-      <c r="B16" s="320" t="s">
+      <c r="B16" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C16" s="320" t="s">
+      <c r="C16" s="323" t="s">
         <v>496</v>
       </c>
-      <c r="D16" s="321" t="n">
+      <c r="D16" s="324" t="n">
         <v>67.7</v>
       </c>
-      <c r="E16" s="342" t="n">
-        <v>70.89</v>
-      </c>
-      <c r="F16" s="342" t="n">
-        <v>74.07</v>
-      </c>
-      <c r="G16" s="342" t="n">
-        <v>77.26</v>
-      </c>
-      <c r="H16" s="342" t="n">
-        <v>80.44</v>
-      </c>
-      <c r="I16" s="342" t="n">
-        <v>83.63</v>
-      </c>
-      <c r="J16" s="342" t="n">
-        <v>86.81</v>
-      </c>
-      <c r="K16" s="342" t="n">
-        <v>90</v>
+      <c r="E16" s="348" t="n">
+        <v>69.51</v>
+      </c>
+      <c r="F16" s="348" t="n">
+        <v>71.52</v>
+      </c>
+      <c r="G16" s="348" t="n">
+        <v>72.9</v>
+      </c>
+      <c r="H16" s="348" t="n">
+        <v>73.14</v>
+      </c>
+      <c r="I16" s="348" t="n">
+        <v>74.48</v>
+      </c>
+      <c r="J16" s="348" t="n">
+        <v>75.68</v>
+      </c>
+      <c r="K16" s="348" t="n">
+        <v>76.52</v>
       </c>
       <c r="L16" s="186"/>
       <c r="M16" s="186"/>
@@ -17971,35 +18157,35 @@
     </row>
     <row r="17" outlineLevel="1" hidden="0">
       <c r="A17" s="186"/>
-      <c r="B17" s="320" t="s">
+      <c r="B17" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C17" s="320" t="s">
+      <c r="C17" s="323" t="s">
         <v>496</v>
       </c>
-      <c r="D17" s="322" t="n">
+      <c r="D17" s="325" t="n">
         <v>67.7</v>
       </c>
-      <c r="E17" s="343" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="F17" s="343" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="G17" s="343" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="H17" s="343" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="I17" s="343" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="J17" s="343" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="K17" s="343" t="n">
-        <v>67.7</v>
+      <c r="E17" s="349" t="n">
+        <v>69.51</v>
+      </c>
+      <c r="F17" s="349" t="n">
+        <v>71.52</v>
+      </c>
+      <c r="G17" s="349" t="n">
+        <v>72.9</v>
+      </c>
+      <c r="H17" s="349" t="n">
+        <v>73.14</v>
+      </c>
+      <c r="I17" s="349" t="n">
+        <v>74.48</v>
+      </c>
+      <c r="J17" s="349" t="n">
+        <v>75.68</v>
+      </c>
+      <c r="K17" s="349" t="n">
+        <v>76.52</v>
       </c>
       <c r="L17" s="186"/>
       <c r="M17" s="186"/>
@@ -18019,28 +18205,28 @@
       <c r="C18" s="284" t="s">
         <v>500</v>
       </c>
-      <c r="D18" s="323" t="n">
+      <c r="D18" s="326" t="n">
         <v>69</v>
       </c>
-      <c r="E18" s="344" t="n">
+      <c r="E18" s="350" t="n">
         <v>73</v>
       </c>
-      <c r="F18" s="344" t="n">
+      <c r="F18" s="350" t="n">
         <v>61</v>
       </c>
-      <c r="G18" s="344" t="n">
+      <c r="G18" s="350" t="n">
         <v>61</v>
       </c>
-      <c r="H18" s="344" t="n">
+      <c r="H18" s="350" t="n">
         <v>61</v>
       </c>
-      <c r="I18" s="344" t="n">
+      <c r="I18" s="350" t="n">
         <v>61</v>
       </c>
-      <c r="J18" s="344" t="n">
+      <c r="J18" s="350" t="n">
         <v>61</v>
       </c>
-      <c r="K18" s="344" t="n">
+      <c r="K18" s="350" t="n">
         <v>61</v>
       </c>
       <c r="L18" s="186"/>
@@ -18055,35 +18241,35 @@
     </row>
     <row r="19" outlineLevel="1" hidden="0">
       <c r="A19" s="186"/>
-      <c r="B19" s="320" t="s">
+      <c r="B19" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C19" s="320" t="s">
+      <c r="C19" s="323" t="s">
         <v>500</v>
       </c>
-      <c r="D19" s="320" t="n">
+      <c r="D19" s="323" t="n">
         <v>69</v>
       </c>
-      <c r="E19" s="320" t="n">
+      <c r="E19" s="323" t="n">
         <v>73</v>
       </c>
-      <c r="F19" s="320" t="n">
-        <v>75</v>
-      </c>
-      <c r="G19" s="345" t="n">
-        <v>78</v>
-      </c>
-      <c r="H19" s="345" t="n">
-        <v>81</v>
-      </c>
-      <c r="I19" s="345" t="n">
-        <v>84</v>
-      </c>
-      <c r="J19" s="345" t="n">
-        <v>87</v>
-      </c>
-      <c r="K19" s="345" t="n">
-        <v>90</v>
+      <c r="F19" s="323" t="n">
+        <v>61</v>
+      </c>
+      <c r="G19" s="351" t="n">
+        <v>61</v>
+      </c>
+      <c r="H19" s="351" t="n">
+        <v>59</v>
+      </c>
+      <c r="I19" s="351" t="n">
+        <v>57</v>
+      </c>
+      <c r="J19" s="351" t="n">
+        <v>55</v>
+      </c>
+      <c r="K19" s="351" t="n">
+        <v>53</v>
       </c>
       <c r="L19" s="186"/>
       <c r="M19" s="186"/>
@@ -18097,35 +18283,35 @@
     </row>
     <row r="20" outlineLevel="1" hidden="0">
       <c r="A20" s="186"/>
-      <c r="B20" s="320" t="s">
+      <c r="B20" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C20" s="320" t="s">
+      <c r="C20" s="323" t="s">
         <v>500</v>
       </c>
-      <c r="D20" s="320" t="n">
+      <c r="D20" s="323" t="n">
         <v>69</v>
       </c>
-      <c r="E20" s="320" t="n">
-        <v>69</v>
-      </c>
-      <c r="F20" s="320" t="n">
-        <v>69</v>
-      </c>
-      <c r="G20" s="346" t="n">
-        <v>69</v>
-      </c>
-      <c r="H20" s="346" t="n">
-        <v>69</v>
-      </c>
-      <c r="I20" s="346" t="n">
-        <v>69</v>
-      </c>
-      <c r="J20" s="346" t="n">
-        <v>69</v>
-      </c>
-      <c r="K20" s="346" t="n">
-        <v>69</v>
+      <c r="E20" s="323" t="n">
+        <v>73</v>
+      </c>
+      <c r="F20" s="323" t="n">
+        <v>61</v>
+      </c>
+      <c r="G20" s="352" t="n">
+        <v>61</v>
+      </c>
+      <c r="H20" s="352" t="n">
+        <v>61</v>
+      </c>
+      <c r="I20" s="352" t="n">
+        <v>61</v>
+      </c>
+      <c r="J20" s="352" t="n">
+        <v>61</v>
+      </c>
+      <c r="K20" s="352" t="n">
+        <v>61</v>
       </c>
       <c r="L20" s="186"/>
       <c r="M20" s="186"/>
@@ -18145,28 +18331,28 @@
       <c r="C21" s="284" t="s">
         <v>504</v>
       </c>
-      <c r="D21" s="320" t="n">
+      <c r="D21" s="323" t="n">
         <v>9.21</v>
       </c>
-      <c r="E21" s="320" t="n">
+      <c r="E21" s="323" t="n">
         <v>9.53</v>
       </c>
-      <c r="F21" s="320" t="n">
-        <v>9.64</v>
-      </c>
-      <c r="G21" s="347" t="n">
+      <c r="F21" s="323" t="n">
+        <v>9.22</v>
+      </c>
+      <c r="G21" s="353" t="n">
         <v>10.57</v>
       </c>
-      <c r="H21" s="347" t="n">
+      <c r="H21" s="353" t="n">
         <v>10.82</v>
       </c>
-      <c r="I21" s="347" t="n">
+      <c r="I21" s="353" t="n">
         <v>11.47</v>
       </c>
-      <c r="J21" s="347" t="n">
+      <c r="J21" s="353" t="n">
         <v>12.02</v>
       </c>
-      <c r="K21" s="347" t="n">
+      <c r="K21" s="353" t="n">
         <v>12.62</v>
       </c>
       <c r="L21" s="186"/>
@@ -18181,35 +18367,35 @@
     </row>
     <row r="22" outlineLevel="1" hidden="0">
       <c r="A22" s="186"/>
-      <c r="B22" s="320" t="s">
+      <c r="B22" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C22" s="320" t="s">
+      <c r="C22" s="323" t="s">
         <v>504</v>
       </c>
-      <c r="D22" s="324" t="n">
+      <c r="D22" s="327" t="n">
         <v>9.21</v>
       </c>
-      <c r="E22" s="324" t="n">
-        <v>20.79</v>
-      </c>
-      <c r="F22" s="348" t="n">
-        <v>32.36</v>
-      </c>
-      <c r="G22" s="348" t="n">
-        <v>43.94</v>
-      </c>
-      <c r="H22" s="348" t="n">
-        <v>55.52</v>
-      </c>
-      <c r="I22" s="348" t="n">
-        <v>67.1</v>
-      </c>
-      <c r="J22" s="348" t="n">
-        <v>78.67</v>
-      </c>
-      <c r="K22" s="348" t="n">
-        <v>90.25</v>
+      <c r="E22" s="327" t="n">
+        <v>9.53</v>
+      </c>
+      <c r="F22" s="327" t="n">
+        <v>9.22</v>
+      </c>
+      <c r="G22" s="354" t="n">
+        <v>9.22</v>
+      </c>
+      <c r="H22" s="354" t="n">
+        <v>9.73</v>
+      </c>
+      <c r="I22" s="354" t="n">
+        <v>10.25</v>
+      </c>
+      <c r="J22" s="354" t="n">
+        <v>10.76</v>
+      </c>
+      <c r="K22" s="354" t="n">
+        <v>11.28</v>
       </c>
       <c r="L22" s="186"/>
       <c r="M22" s="186"/>
@@ -18223,35 +18409,35 @@
     </row>
     <row r="23" outlineLevel="1" hidden="0">
       <c r="A23" s="186"/>
-      <c r="B23" s="320" t="s">
+      <c r="B23" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C23" s="320" t="s">
+      <c r="C23" s="323" t="s">
         <v>504</v>
       </c>
-      <c r="D23" s="325" t="n">
+      <c r="D23" s="328" t="n">
         <v>9.21</v>
       </c>
-      <c r="E23" s="325" t="n">
-        <v>9.21</v>
-      </c>
-      <c r="F23" s="349" t="n">
-        <v>9.21</v>
-      </c>
-      <c r="G23" s="349" t="n">
-        <v>9.21</v>
-      </c>
-      <c r="H23" s="349" t="n">
-        <v>9.21</v>
-      </c>
-      <c r="I23" s="349" t="n">
-        <v>9.21</v>
-      </c>
-      <c r="J23" s="349" t="n">
-        <v>9.21</v>
-      </c>
-      <c r="K23" s="349" t="n">
-        <v>9.21</v>
+      <c r="E23" s="328" t="n">
+        <v>9.53</v>
+      </c>
+      <c r="F23" s="328" t="n">
+        <v>9.22</v>
+      </c>
+      <c r="G23" s="355" t="n">
+        <v>10.57</v>
+      </c>
+      <c r="H23" s="355" t="n">
+        <v>10.82</v>
+      </c>
+      <c r="I23" s="355" t="n">
+        <v>11.47</v>
+      </c>
+      <c r="J23" s="355" t="n">
+        <v>12.02</v>
+      </c>
+      <c r="K23" s="355" t="n">
+        <v>12.62</v>
       </c>
       <c r="L23" s="186"/>
       <c r="M23" s="186"/>
@@ -18271,14 +18457,14 @@
       <c r="C24" s="284" t="s">
         <v>508</v>
       </c>
-      <c r="D24" s="326"/>
-      <c r="E24" s="326"/>
-      <c r="F24" s="350"/>
-      <c r="G24" s="350"/>
-      <c r="H24" s="350"/>
-      <c r="I24" s="350"/>
-      <c r="J24" s="350"/>
-      <c r="K24" s="350"/>
+      <c r="D24" s="329"/>
+      <c r="E24" s="329"/>
+      <c r="F24" s="329"/>
+      <c r="G24" s="356"/>
+      <c r="H24" s="356"/>
+      <c r="I24" s="356"/>
+      <c r="J24" s="356"/>
+      <c r="K24" s="356"/>
       <c r="L24" s="186"/>
       <c r="M24" s="186"/>
       <c r="N24" s="186"/>
@@ -18291,20 +18477,20 @@
     </row>
     <row r="25" outlineLevel="1" hidden="0">
       <c r="A25" s="186"/>
-      <c r="B25" s="320" t="s">
+      <c r="B25" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C25" s="320" t="s">
+      <c r="C25" s="323" t="s">
         <v>508</v>
       </c>
-      <c r="D25" s="320"/>
-      <c r="E25" s="320"/>
-      <c r="F25" s="320"/>
-      <c r="G25" s="320"/>
-      <c r="H25" s="320"/>
-      <c r="I25" s="320"/>
-      <c r="J25" s="320"/>
-      <c r="K25" s="320"/>
+      <c r="D25" s="323"/>
+      <c r="E25" s="323"/>
+      <c r="F25" s="323"/>
+      <c r="G25" s="323"/>
+      <c r="H25" s="323"/>
+      <c r="I25" s="323"/>
+      <c r="J25" s="323"/>
+      <c r="K25" s="323"/>
       <c r="L25" s="186"/>
       <c r="M25" s="186"/>
       <c r="N25" s="186"/>
@@ -18317,20 +18503,20 @@
     </row>
     <row r="26" outlineLevel="1" hidden="0">
       <c r="A26" s="186"/>
-      <c r="B26" s="320" t="s">
+      <c r="B26" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C26" s="320" t="s">
+      <c r="C26" s="323" t="s">
         <v>508</v>
       </c>
-      <c r="D26" s="320"/>
-      <c r="E26" s="320"/>
-      <c r="F26" s="351"/>
-      <c r="G26" s="351"/>
-      <c r="H26" s="351"/>
-      <c r="I26" s="351"/>
-      <c r="J26" s="351"/>
-      <c r="K26" s="351"/>
+      <c r="D26" s="323"/>
+      <c r="E26" s="323"/>
+      <c r="F26" s="323"/>
+      <c r="G26" s="357"/>
+      <c r="H26" s="357"/>
+      <c r="I26" s="357"/>
+      <c r="J26" s="357"/>
+      <c r="K26" s="357"/>
       <c r="L26" s="186"/>
       <c r="M26" s="186"/>
       <c r="N26" s="186"/>
@@ -18349,28 +18535,28 @@
       <c r="C27" s="284" t="s">
         <v>513</v>
       </c>
-      <c r="D27" s="320" t="n">
+      <c r="D27" s="323" t="n">
         <v>47.39</v>
       </c>
-      <c r="E27" s="320" t="n">
+      <c r="E27" s="323" t="n">
         <v>49.01</v>
       </c>
-      <c r="F27" s="352" t="n">
-        <v>50.61</v>
-      </c>
-      <c r="G27" s="352" t="n">
+      <c r="F27" s="323" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="G27" s="358" t="n">
         <v>52.22</v>
       </c>
-      <c r="H27" s="352" t="n">
+      <c r="H27" s="358" t="n">
         <v>53.83</v>
       </c>
-      <c r="I27" s="352" t="n">
+      <c r="I27" s="358" t="n">
         <v>55.43</v>
       </c>
-      <c r="J27" s="352" t="n">
+      <c r="J27" s="358" t="n">
         <v>57.02</v>
       </c>
-      <c r="K27" s="352" t="n">
+      <c r="K27" s="358" t="n">
         <v>58.6</v>
       </c>
       <c r="L27" s="186"/>
@@ -18385,20 +18571,36 @@
     </row>
     <row r="28" outlineLevel="1" hidden="0">
       <c r="A28" s="186"/>
-      <c r="B28" s="320" t="s">
+      <c r="B28" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C28" s="320" t="s">
+      <c r="C28" s="323" t="s">
         <v>513</v>
       </c>
-      <c r="D28" s="320"/>
-      <c r="E28" s="320"/>
-      <c r="F28" s="353"/>
-      <c r="G28" s="353"/>
-      <c r="H28" s="353"/>
-      <c r="I28" s="353"/>
-      <c r="J28" s="353"/>
-      <c r="K28" s="353"/>
+      <c r="D28" s="323" t="n">
+        <v>47.39</v>
+      </c>
+      <c r="E28" s="323" t="n">
+        <v>49.01</v>
+      </c>
+      <c r="F28" s="323" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="G28" s="359" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="H28" s="359" t="n">
+        <v>52.1</v>
+      </c>
+      <c r="I28" s="359" t="n">
+        <v>53.7</v>
+      </c>
+      <c r="J28" s="359" t="n">
+        <v>55.3</v>
+      </c>
+      <c r="K28" s="359" t="n">
+        <v>56.9</v>
+      </c>
       <c r="L28" s="186"/>
       <c r="M28" s="186"/>
       <c r="N28" s="186"/>
@@ -18411,35 +18613,35 @@
     </row>
     <row r="29" outlineLevel="1" hidden="0">
       <c r="A29" s="186"/>
-      <c r="B29" s="320" t="s">
+      <c r="B29" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C29" s="320" t="s">
+      <c r="C29" s="323" t="s">
         <v>513</v>
       </c>
-      <c r="D29" s="320" t="n">
+      <c r="D29" s="323" t="n">
         <v>47.39</v>
       </c>
-      <c r="E29" s="320" t="n">
-        <v>47.39</v>
-      </c>
-      <c r="F29" s="354" t="n">
-        <v>47.39</v>
-      </c>
-      <c r="G29" s="354" t="n">
-        <v>47.39</v>
-      </c>
-      <c r="H29" s="354" t="n">
-        <v>47.39</v>
-      </c>
-      <c r="I29" s="354" t="n">
-        <v>47.39</v>
-      </c>
-      <c r="J29" s="354" t="n">
-        <v>47.39</v>
-      </c>
-      <c r="K29" s="354" t="n">
-        <v>47.39</v>
+      <c r="E29" s="323" t="n">
+        <v>49.01</v>
+      </c>
+      <c r="F29" s="360" t="n">
+        <v>50.5</v>
+      </c>
+      <c r="G29" s="360" t="n">
+        <v>52.22</v>
+      </c>
+      <c r="H29" s="360" t="n">
+        <v>53.83</v>
+      </c>
+      <c r="I29" s="360" t="n">
+        <v>55.43</v>
+      </c>
+      <c r="J29" s="360" t="n">
+        <v>57.02</v>
+      </c>
+      <c r="K29" s="360" t="n">
+        <v>58.6</v>
       </c>
       <c r="L29" s="186"/>
       <c r="M29" s="186"/>
@@ -18459,28 +18661,28 @@
       <c r="C30" s="284" t="s">
         <v>517</v>
       </c>
-      <c r="D30" s="320" t="n">
+      <c r="D30" s="323" t="n">
         <v>40.14</v>
       </c>
-      <c r="E30" s="320" t="n">
+      <c r="E30" s="323" t="n">
         <v>40.4</v>
       </c>
-      <c r="F30" s="355" t="n">
+      <c r="F30" s="361" t="n">
         <v>40.65</v>
       </c>
-      <c r="G30" s="355" t="n">
+      <c r="G30" s="361" t="n">
         <v>40.91</v>
       </c>
-      <c r="H30" s="355" t="n">
+      <c r="H30" s="361" t="n">
         <v>41.17</v>
       </c>
-      <c r="I30" s="355" t="n">
+      <c r="I30" s="361" t="n">
         <v>41.43</v>
       </c>
-      <c r="J30" s="355" t="n">
+      <c r="J30" s="361" t="n">
         <v>41.7</v>
       </c>
-      <c r="K30" s="355" t="n">
+      <c r="K30" s="361" t="n">
         <v>41.96</v>
       </c>
       <c r="L30" s="186"/>
@@ -18495,34 +18697,34 @@
     </row>
     <row r="31" outlineLevel="1" hidden="0">
       <c r="A31" s="186"/>
-      <c r="B31" s="320" t="s">
+      <c r="B31" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C31" s="320" t="s">
+      <c r="C31" s="323" t="s">
         <v>517</v>
       </c>
-      <c r="D31" s="356" t="n">
-        <v>43.8</v>
-      </c>
-      <c r="E31" s="356" t="n">
-        <v>44.03</v>
-      </c>
-      <c r="F31" s="356" t="n">
-        <v>44.31</v>
-      </c>
-      <c r="G31" s="356" t="n">
-        <v>44.6</v>
-      </c>
-      <c r="H31" s="356" t="n">
-        <v>44.88</v>
-      </c>
-      <c r="I31" s="356" t="n">
-        <v>45.16</v>
-      </c>
-      <c r="J31" s="356" t="n">
+      <c r="D31" s="323" t="n">
+        <v>40.14</v>
+      </c>
+      <c r="E31" s="323" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="F31" s="362" t="n">
+        <v>40.65</v>
+      </c>
+      <c r="G31" s="362" t="n">
+        <v>40.91</v>
+      </c>
+      <c r="H31" s="362" t="n">
+        <v>41.17</v>
+      </c>
+      <c r="I31" s="362" t="n">
+        <v>41.43</v>
+      </c>
+      <c r="J31" s="362" t="n">
         <v>41.7</v>
       </c>
-      <c r="K31" s="356" t="n">
+      <c r="K31" s="362" t="n">
         <v>41.96</v>
       </c>
       <c r="L31" s="186"/>
@@ -18537,35 +18739,35 @@
     </row>
     <row r="32" outlineLevel="1" hidden="0">
       <c r="A32" s="186"/>
-      <c r="B32" s="320" t="s">
+      <c r="B32" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C32" s="320" t="s">
+      <c r="C32" s="323" t="s">
         <v>517</v>
       </c>
-      <c r="D32" s="357" t="n">
+      <c r="D32" s="363" t="n">
         <v>40.14</v>
       </c>
-      <c r="E32" s="357" t="n">
-        <v>40.14</v>
-      </c>
-      <c r="F32" s="357" t="n">
-        <v>40.14</v>
-      </c>
-      <c r="G32" s="357" t="n">
-        <v>40.14</v>
-      </c>
-      <c r="H32" s="357" t="n">
-        <v>40.14</v>
-      </c>
-      <c r="I32" s="357" t="n">
-        <v>40.14</v>
-      </c>
-      <c r="J32" s="357" t="n">
-        <v>40.14</v>
-      </c>
-      <c r="K32" s="357" t="n">
-        <v>40.14</v>
+      <c r="E32" s="363" t="n">
+        <v>40.4</v>
+      </c>
+      <c r="F32" s="363" t="n">
+        <v>40.65</v>
+      </c>
+      <c r="G32" s="363" t="n">
+        <v>40.91</v>
+      </c>
+      <c r="H32" s="363" t="n">
+        <v>41.17</v>
+      </c>
+      <c r="I32" s="363" t="n">
+        <v>41.43</v>
+      </c>
+      <c r="J32" s="363" t="n">
+        <v>41.7</v>
+      </c>
+      <c r="K32" s="363" t="n">
+        <v>41.96</v>
       </c>
       <c r="L32" s="186"/>
       <c r="M32" s="186"/>
@@ -18585,28 +18787,28 @@
       <c r="C33" s="284" t="s">
         <v>522</v>
       </c>
-      <c r="D33" s="358" t="n">
+      <c r="D33" s="364" t="n">
         <v>5.47</v>
       </c>
-      <c r="E33" s="358" t="n">
+      <c r="E33" s="364" t="n">
         <v>5.49</v>
       </c>
-      <c r="F33" s="358" t="n">
+      <c r="F33" s="364" t="n">
         <v>5.52</v>
       </c>
-      <c r="G33" s="358" t="n">
+      <c r="G33" s="364" t="n">
         <v>5.54</v>
       </c>
-      <c r="H33" s="358" t="n">
+      <c r="H33" s="364" t="n">
         <v>5.57</v>
       </c>
-      <c r="I33" s="358" t="n">
+      <c r="I33" s="364" t="n">
         <v>5.59</v>
       </c>
-      <c r="J33" s="358" t="n">
+      <c r="J33" s="364" t="n">
         <v>5.62</v>
       </c>
-      <c r="K33" s="358" t="n">
+      <c r="K33" s="364" t="n">
         <v>5.65</v>
       </c>
       <c r="L33" s="186"/>
@@ -18621,34 +18823,34 @@
     </row>
     <row r="34" outlineLevel="1" hidden="0">
       <c r="A34" s="186"/>
-      <c r="B34" s="320" t="s">
+      <c r="B34" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C34" s="320" t="s">
+      <c r="C34" s="323" t="s">
         <v>522</v>
       </c>
-      <c r="D34" s="320" t="n">
+      <c r="D34" s="365" t="n">
         <v>5.47</v>
       </c>
-      <c r="E34" s="320" t="n">
+      <c r="E34" s="365" t="n">
         <v>5.49</v>
       </c>
-      <c r="F34" s="359" t="n">
+      <c r="F34" s="365" t="n">
         <v>5.52</v>
       </c>
-      <c r="G34" s="383" t="n">
+      <c r="G34" s="365" t="n">
         <v>5.54</v>
       </c>
-      <c r="H34" s="383" t="n">
+      <c r="H34" s="365" t="n">
         <v>5.57</v>
       </c>
-      <c r="I34" s="359" t="n">
+      <c r="I34" s="365" t="n">
         <v>5.59</v>
       </c>
-      <c r="J34" s="383" t="n">
+      <c r="J34" s="365" t="n">
         <v>5.62</v>
       </c>
-      <c r="K34" s="359" t="n">
+      <c r="K34" s="365" t="n">
         <v>5.65</v>
       </c>
       <c r="L34" s="186"/>
@@ -18663,35 +18865,35 @@
     </row>
     <row r="35" outlineLevel="1" hidden="0">
       <c r="A35" s="186"/>
-      <c r="B35" s="320" t="s">
+      <c r="B35" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C35" s="320" t="s">
+      <c r="C35" s="323" t="s">
         <v>522</v>
       </c>
-      <c r="D35" s="320" t="n">
+      <c r="D35" s="323" t="n">
         <v>5.47</v>
       </c>
-      <c r="E35" s="320" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="F35" s="360" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="G35" s="384" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="H35" s="384" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="I35" s="360" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="J35" s="384" t="n">
-        <v>5.47</v>
-      </c>
-      <c r="K35" s="360" t="n">
-        <v>5.47</v>
+      <c r="E35" s="323" t="n">
+        <v>5.49</v>
+      </c>
+      <c r="F35" s="366" t="n">
+        <v>5.52</v>
+      </c>
+      <c r="G35" s="393" t="n">
+        <v>5.54</v>
+      </c>
+      <c r="H35" s="393" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="I35" s="366" t="n">
+        <v>5.59</v>
+      </c>
+      <c r="J35" s="393" t="n">
+        <v>5.62</v>
+      </c>
+      <c r="K35" s="366" t="n">
+        <v>5.65</v>
       </c>
       <c r="L35" s="186"/>
       <c r="M35" s="186"/>
@@ -18711,28 +18913,28 @@
       <c r="C36" s="284" t="s">
         <v>526</v>
       </c>
-      <c r="D36" s="320" t="n">
+      <c r="D36" s="323" t="n">
         <v>24.35</v>
       </c>
-      <c r="E36" s="320" t="n">
+      <c r="E36" s="323" t="n">
         <v>23.8</v>
       </c>
-      <c r="F36" s="361" t="n">
+      <c r="F36" s="367" t="n">
         <v>23.3</v>
       </c>
-      <c r="G36" s="385" t="n">
+      <c r="G36" s="394" t="n">
         <v>22.8</v>
       </c>
-      <c r="H36" s="385" t="n">
+      <c r="H36" s="394" t="n">
         <v>22.3</v>
       </c>
-      <c r="I36" s="361" t="n">
+      <c r="I36" s="367" t="n">
         <v>21.8</v>
       </c>
-      <c r="J36" s="385" t="n">
+      <c r="J36" s="394" t="n">
         <v>21.4</v>
       </c>
-      <c r="K36" s="361" t="n">
+      <c r="K36" s="367" t="n">
         <v>21</v>
       </c>
       <c r="L36" s="186"/>
@@ -18747,35 +18949,35 @@
     </row>
     <row r="37" outlineLevel="1" hidden="0">
       <c r="A37" s="186"/>
-      <c r="B37" s="320" t="s">
+      <c r="B37" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C37" s="320" t="s">
+      <c r="C37" s="323" t="s">
         <v>526</v>
       </c>
-      <c r="D37" s="327" t="n">
-        <v>25.45</v>
-      </c>
-      <c r="E37" s="327" t="n">
-        <v>24.82</v>
-      </c>
-      <c r="F37" s="362" t="n">
-        <v>24.31</v>
-      </c>
-      <c r="G37" s="362" t="n">
-        <v>23.8</v>
-      </c>
-      <c r="H37" s="362" t="n">
-        <v>23.29</v>
-      </c>
-      <c r="I37" s="362" t="n">
-        <v>22.78</v>
-      </c>
-      <c r="J37" s="362" t="n">
-        <v>23.98</v>
-      </c>
-      <c r="K37" s="362" t="n">
-        <v>23.53</v>
+      <c r="D37" s="323" t="n">
+        <v>75.65</v>
+      </c>
+      <c r="E37" s="323" t="n">
+        <v>76.2</v>
+      </c>
+      <c r="F37" s="368" t="n">
+        <v>76.7</v>
+      </c>
+      <c r="G37" s="395" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="H37" s="395" t="n">
+        <v>77.7</v>
+      </c>
+      <c r="I37" s="368" t="n">
+        <v>78.2</v>
+      </c>
+      <c r="J37" s="395" t="n">
+        <v>78.6</v>
+      </c>
+      <c r="K37" s="368" t="n">
+        <v>79</v>
       </c>
       <c r="L37" s="186"/>
       <c r="M37" s="186"/>
@@ -18789,35 +18991,35 @@
     </row>
     <row r="38" outlineLevel="1" hidden="0">
       <c r="A38" s="186"/>
-      <c r="B38" s="320" t="s">
+      <c r="B38" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C38" s="320" t="s">
+      <c r="C38" s="323" t="s">
         <v>526</v>
       </c>
-      <c r="D38" s="328" t="n">
+      <c r="D38" s="330" t="n">
         <v>24.35</v>
       </c>
-      <c r="E38" s="328" t="n">
-        <v>24.35</v>
-      </c>
-      <c r="F38" s="363" t="n">
-        <v>24.35</v>
-      </c>
-      <c r="G38" s="363" t="n">
-        <v>24.35</v>
-      </c>
-      <c r="H38" s="363" t="n">
-        <v>24.35</v>
-      </c>
-      <c r="I38" s="363" t="n">
-        <v>24.35</v>
-      </c>
-      <c r="J38" s="363" t="n">
-        <v>24.35</v>
-      </c>
-      <c r="K38" s="363" t="n">
-        <v>24.35</v>
+      <c r="E38" s="330" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="F38" s="330" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="G38" s="369" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="H38" s="369" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="I38" s="369" t="n">
+        <v>21.8</v>
+      </c>
+      <c r="J38" s="369" t="n">
+        <v>21.4</v>
+      </c>
+      <c r="K38" s="369" t="n">
+        <v>21</v>
       </c>
       <c r="L38" s="186"/>
       <c r="M38" s="186"/>
@@ -18837,28 +19039,28 @@
       <c r="C39" s="284" t="s">
         <v>531</v>
       </c>
-      <c r="D39" s="329" t="n">
+      <c r="D39" s="331" t="n">
         <v>3.96</v>
       </c>
-      <c r="E39" s="329" t="n">
+      <c r="E39" s="331" t="n">
         <v>3.81</v>
       </c>
-      <c r="F39" s="364" t="n">
-        <v>3.67</v>
-      </c>
-      <c r="G39" s="364" t="n">
+      <c r="F39" s="331" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="G39" s="370" t="n">
         <v>3.52</v>
       </c>
-      <c r="H39" s="364" t="n">
+      <c r="H39" s="370" t="n">
         <v>3.37</v>
       </c>
-      <c r="I39" s="364" t="n">
+      <c r="I39" s="370" t="n">
         <v>3.23</v>
       </c>
-      <c r="J39" s="364" t="n">
+      <c r="J39" s="370" t="n">
         <v>3.1</v>
       </c>
-      <c r="K39" s="364" t="n">
+      <c r="K39" s="370" t="n">
         <v>2.97</v>
       </c>
       <c r="L39" s="186"/>
@@ -18873,35 +19075,35 @@
     </row>
     <row r="40" outlineLevel="1" hidden="0">
       <c r="A40" s="186"/>
-      <c r="B40" s="320" t="s">
+      <c r="B40" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C40" s="320" t="s">
+      <c r="C40" s="323" t="s">
         <v>531</v>
       </c>
-      <c r="D40" s="365" t="n">
+      <c r="D40" s="332" t="n">
         <v>3.96</v>
       </c>
-      <c r="E40" s="365" t="n">
-        <v>4.32</v>
-      </c>
-      <c r="F40" s="365" t="n">
-        <v>4.68</v>
-      </c>
-      <c r="G40" s="365" t="n">
-        <v>5.04</v>
-      </c>
-      <c r="H40" s="365" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="I40" s="365" t="n">
-        <v>5.76</v>
-      </c>
-      <c r="J40" s="365" t="n">
-        <v>6.12</v>
-      </c>
-      <c r="K40" s="365" t="n">
-        <v>6.48</v>
+      <c r="E40" s="332" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="F40" s="332" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="G40" s="371" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="H40" s="371" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="I40" s="371" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="J40" s="371" t="n">
+        <v>2.93</v>
+      </c>
+      <c r="K40" s="371" t="n">
+        <v>2.79</v>
       </c>
       <c r="L40" s="186"/>
       <c r="M40" s="186"/>
@@ -18915,35 +19117,35 @@
     </row>
     <row r="41" outlineLevel="1" hidden="0">
       <c r="A41" s="186"/>
-      <c r="B41" s="320" t="s">
+      <c r="B41" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C41" s="320" t="s">
+      <c r="C41" s="323" t="s">
         <v>531</v>
       </c>
-      <c r="D41" s="366" t="n">
+      <c r="D41" s="372" t="n">
         <v>3.96</v>
       </c>
-      <c r="E41" s="366" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="F41" s="366" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="G41" s="366" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="H41" s="366" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="I41" s="366" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="J41" s="366" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="K41" s="366" t="n">
-        <v>3.96</v>
+      <c r="E41" s="372" t="n">
+        <v>3.81</v>
+      </c>
+      <c r="F41" s="372" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="G41" s="372" t="n">
+        <v>3.52</v>
+      </c>
+      <c r="H41" s="372" t="n">
+        <v>3.37</v>
+      </c>
+      <c r="I41" s="372" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="J41" s="372" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="K41" s="372" t="n">
+        <v>2.97</v>
       </c>
       <c r="L41" s="186"/>
       <c r="M41" s="186"/>
@@ -18963,28 +19165,28 @@
       <c r="C42" s="284" t="s">
         <v>535</v>
       </c>
-      <c r="D42" s="367" t="n">
+      <c r="D42" s="373" t="n">
         <v>7.24</v>
       </c>
-      <c r="E42" s="367" t="n">
+      <c r="E42" s="373" t="n">
         <v>7.24</v>
       </c>
-      <c r="F42" s="367" t="n">
+      <c r="F42" s="373" t="n">
         <v>7.24</v>
       </c>
-      <c r="G42" s="367" t="n">
+      <c r="G42" s="373" t="n">
         <v>7.97</v>
       </c>
-      <c r="H42" s="367" t="n">
+      <c r="H42" s="373" t="n">
         <v>8.7</v>
       </c>
-      <c r="I42" s="367" t="n">
+      <c r="I42" s="373" t="n">
         <v>9.43</v>
       </c>
-      <c r="J42" s="367" t="n">
+      <c r="J42" s="373" t="n">
         <v>10.16</v>
       </c>
-      <c r="K42" s="367" t="n">
+      <c r="K42" s="373" t="n">
         <v>10.89</v>
       </c>
       <c r="L42" s="186"/>
@@ -18999,35 +19201,35 @@
     </row>
     <row r="43" outlineLevel="1" hidden="0">
       <c r="A43" s="186"/>
-      <c r="B43" s="320" t="s">
+      <c r="B43" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C43" s="320" t="s">
+      <c r="C43" s="323" t="s">
         <v>535</v>
       </c>
-      <c r="D43" s="368" t="n">
+      <c r="D43" s="374" t="n">
         <v>7.24</v>
       </c>
-      <c r="E43" s="368" t="n">
-        <v>11.78</v>
-      </c>
-      <c r="F43" s="368" t="n">
-        <v>16.32</v>
-      </c>
-      <c r="G43" s="368" t="n">
-        <v>20.86</v>
-      </c>
-      <c r="H43" s="368" t="n">
-        <v>25.4</v>
-      </c>
-      <c r="I43" s="368" t="n">
-        <v>29.94</v>
-      </c>
-      <c r="J43" s="368" t="n">
-        <v>34.48</v>
-      </c>
-      <c r="K43" s="368" t="n">
-        <v>39.02</v>
+      <c r="E43" s="374" t="n">
+        <v>7.24</v>
+      </c>
+      <c r="F43" s="374" t="n">
+        <v>7.24</v>
+      </c>
+      <c r="G43" s="374" t="n">
+        <v>7.97</v>
+      </c>
+      <c r="H43" s="374" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="I43" s="374" t="n">
+        <v>9.43</v>
+      </c>
+      <c r="J43" s="374" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="K43" s="374" t="n">
+        <v>10.89</v>
       </c>
       <c r="L43" s="186"/>
       <c r="M43" s="186"/>
@@ -19041,35 +19243,35 @@
     </row>
     <row r="44" outlineLevel="1" hidden="0">
       <c r="A44" s="186"/>
-      <c r="B44" s="320" t="s">
+      <c r="B44" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C44" s="320" t="s">
+      <c r="C44" s="323" t="s">
         <v>535</v>
       </c>
-      <c r="D44" s="369" t="n">
+      <c r="D44" s="375" t="n">
         <v>7.24</v>
       </c>
-      <c r="E44" s="369" t="n">
+      <c r="E44" s="375" t="n">
         <v>7.24</v>
       </c>
-      <c r="F44" s="369" t="n">
+      <c r="F44" s="375" t="n">
         <v>7.24</v>
       </c>
-      <c r="G44" s="369" t="n">
-        <v>7.24</v>
-      </c>
-      <c r="H44" s="369" t="n">
-        <v>7.24</v>
-      </c>
-      <c r="I44" s="369" t="n">
-        <v>7.24</v>
-      </c>
-      <c r="J44" s="369" t="n">
-        <v>7.24</v>
-      </c>
-      <c r="K44" s="369" t="n">
-        <v>7.24</v>
+      <c r="G44" s="375" t="n">
+        <v>7.97</v>
+      </c>
+      <c r="H44" s="375" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="I44" s="375" t="n">
+        <v>9.43</v>
+      </c>
+      <c r="J44" s="375" t="n">
+        <v>10.16</v>
+      </c>
+      <c r="K44" s="375" t="n">
+        <v>10.89</v>
       </c>
       <c r="L44" s="186"/>
       <c r="M44" s="186"/>
@@ -19089,28 +19291,28 @@
       <c r="C45" s="284" t="s">
         <v>539</v>
       </c>
-      <c r="D45" s="370" t="n">
+      <c r="D45" s="376" t="n">
         <v>2.78</v>
       </c>
-      <c r="E45" s="370" t="n">
+      <c r="E45" s="376" t="n">
         <v>2.78</v>
       </c>
-      <c r="F45" s="370" t="n">
+      <c r="F45" s="376" t="n">
         <v>2.78</v>
       </c>
-      <c r="G45" s="370" t="n">
+      <c r="G45" s="376" t="n">
         <v>2.83</v>
       </c>
-      <c r="H45" s="370" t="n">
+      <c r="H45" s="376" t="n">
         <v>2.87</v>
       </c>
-      <c r="I45" s="370" t="n">
+      <c r="I45" s="376" t="n">
         <v>2.91</v>
       </c>
-      <c r="J45" s="370" t="n">
+      <c r="J45" s="376" t="n">
         <v>2.96</v>
       </c>
-      <c r="K45" s="370" t="n">
+      <c r="K45" s="376" t="n">
         <v>3</v>
       </c>
       <c r="L45" s="186"/>
@@ -19125,34 +19327,34 @@
     </row>
     <row r="46" outlineLevel="1" hidden="0">
       <c r="A46" s="186"/>
-      <c r="B46" s="320" t="s">
+      <c r="B46" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C46" s="320" t="s">
+      <c r="C46" s="323" t="s">
         <v>539</v>
       </c>
-      <c r="D46" s="330" t="n">
+      <c r="D46" s="377" t="n">
         <v>2.78</v>
       </c>
-      <c r="E46" s="371" t="n">
+      <c r="E46" s="377" t="n">
         <v>2.78</v>
       </c>
-      <c r="F46" s="371" t="n">
+      <c r="F46" s="377" t="n">
         <v>2.78</v>
       </c>
-      <c r="G46" s="371" t="n">
+      <c r="G46" s="377" t="n">
         <v>2.83</v>
       </c>
-      <c r="H46" s="371" t="n">
+      <c r="H46" s="377" t="n">
         <v>2.87</v>
       </c>
-      <c r="I46" s="371" t="n">
+      <c r="I46" s="377" t="n">
         <v>2.91</v>
       </c>
-      <c r="J46" s="371" t="n">
+      <c r="J46" s="377" t="n">
         <v>2.96</v>
       </c>
-      <c r="K46" s="371" t="n">
+      <c r="K46" s="377" t="n">
         <v>3</v>
       </c>
       <c r="L46" s="186"/>
@@ -19167,35 +19369,35 @@
     </row>
     <row r="47" outlineLevel="1" hidden="0">
       <c r="A47" s="186"/>
-      <c r="B47" s="320" t="s">
+      <c r="B47" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C47" s="320" t="s">
+      <c r="C47" s="323" t="s">
         <v>539</v>
       </c>
-      <c r="D47" s="331" t="n">
+      <c r="D47" s="333" t="n">
         <v>2.78</v>
       </c>
-      <c r="E47" s="372" t="n">
+      <c r="E47" s="378" t="n">
         <v>2.78</v>
       </c>
-      <c r="F47" s="372" t="n">
+      <c r="F47" s="378" t="n">
         <v>2.78</v>
       </c>
-      <c r="G47" s="372" t="n">
-        <v>2.78</v>
-      </c>
-      <c r="H47" s="372" t="n">
-        <v>2.78</v>
-      </c>
-      <c r="I47" s="372" t="n">
-        <v>2.78</v>
-      </c>
-      <c r="J47" s="372" t="n">
-        <v>2.78</v>
-      </c>
-      <c r="K47" s="372" t="n">
-        <v>2.78</v>
+      <c r="G47" s="378" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="H47" s="378" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="I47" s="378" t="n">
+        <v>2.91</v>
+      </c>
+      <c r="J47" s="378" t="n">
+        <v>2.96</v>
+      </c>
+      <c r="K47" s="378" t="n">
+        <v>3</v>
       </c>
       <c r="L47" s="186"/>
       <c r="M47" s="186"/>
@@ -19215,28 +19417,28 @@
       <c r="C48" s="284" t="s">
         <v>543</v>
       </c>
-      <c r="D48" s="332" t="n">
+      <c r="D48" s="334" t="n">
         <v>4.46</v>
       </c>
-      <c r="E48" s="373" t="n">
+      <c r="E48" s="379" t="n">
         <v>4.46</v>
       </c>
-      <c r="F48" s="373" t="n">
+      <c r="F48" s="379" t="n">
         <v>4.46</v>
       </c>
-      <c r="G48" s="373" t="n">
+      <c r="G48" s="379" t="n">
         <v>5.14</v>
       </c>
-      <c r="H48" s="373" t="n">
+      <c r="H48" s="379" t="n">
         <v>5.83</v>
       </c>
-      <c r="I48" s="373" t="n">
+      <c r="I48" s="379" t="n">
         <v>6.52</v>
       </c>
-      <c r="J48" s="373" t="n">
+      <c r="J48" s="379" t="n">
         <v>7.2</v>
       </c>
-      <c r="K48" s="373" t="n">
+      <c r="K48" s="379" t="n">
         <v>7.89</v>
       </c>
       <c r="L48" s="186"/>
@@ -19251,34 +19453,34 @@
     </row>
     <row r="49" outlineLevel="1" hidden="0">
       <c r="A49" s="186"/>
-      <c r="B49" s="320" t="s">
+      <c r="B49" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C49" s="320" t="s">
+      <c r="C49" s="323" t="s">
         <v>543</v>
       </c>
-      <c r="D49" s="320" t="n">
+      <c r="D49" s="335" t="n">
         <v>4.46</v>
       </c>
-      <c r="E49" s="320" t="n">
+      <c r="E49" s="380" t="n">
         <v>4.46</v>
       </c>
-      <c r="F49" s="320" t="n">
+      <c r="F49" s="380" t="n">
         <v>4.46</v>
       </c>
-      <c r="G49" s="320" t="n">
+      <c r="G49" s="380" t="n">
         <v>5.14</v>
       </c>
-      <c r="H49" s="320" t="n">
+      <c r="H49" s="380" t="n">
         <v>5.83</v>
       </c>
-      <c r="I49" s="320" t="n">
+      <c r="I49" s="380" t="n">
         <v>6.52</v>
       </c>
-      <c r="J49" s="320" t="n">
+      <c r="J49" s="380" t="n">
         <v>7.2</v>
       </c>
-      <c r="K49" s="320" t="n">
+      <c r="K49" s="380" t="n">
         <v>7.89</v>
       </c>
       <c r="L49" s="186"/>
@@ -19293,35 +19495,35 @@
     </row>
     <row r="50" outlineLevel="1" hidden="0">
       <c r="A50" s="186"/>
-      <c r="B50" s="320" t="s">
+      <c r="B50" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C50" s="320" t="s">
+      <c r="C50" s="323" t="s">
         <v>543</v>
       </c>
-      <c r="D50" s="374" t="n">
+      <c r="D50" s="336" t="n">
         <v>4.46</v>
       </c>
-      <c r="E50" s="374" t="n">
+      <c r="E50" s="336" t="n">
         <v>4.46</v>
       </c>
-      <c r="F50" s="374" t="n">
+      <c r="F50" s="336" t="n">
         <v>4.46</v>
       </c>
-      <c r="G50" s="374" t="n">
-        <v>4.46</v>
-      </c>
-      <c r="H50" s="374" t="n">
-        <v>4.46</v>
-      </c>
-      <c r="I50" s="374" t="n">
-        <v>4.46</v>
-      </c>
-      <c r="J50" s="374" t="n">
-        <v>4.46</v>
-      </c>
-      <c r="K50" s="374" t="n">
-        <v>4.46</v>
+      <c r="G50" s="381" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="H50" s="381" t="n">
+        <v>5.83</v>
+      </c>
+      <c r="I50" s="381" t="n">
+        <v>6.52</v>
+      </c>
+      <c r="J50" s="381" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="K50" s="381" t="n">
+        <v>7.89</v>
       </c>
       <c r="L50" s="186"/>
       <c r="M50" s="186"/>
@@ -19341,14 +19543,30 @@
       <c r="C51" s="284" t="s">
         <v>547</v>
       </c>
-      <c r="D51" s="375"/>
-      <c r="E51" s="375"/>
-      <c r="F51" s="375"/>
-      <c r="G51" s="375"/>
-      <c r="H51" s="375"/>
-      <c r="I51" s="375"/>
-      <c r="J51" s="375"/>
-      <c r="K51" s="375"/>
+      <c r="D51" s="337" t="n">
+        <v>35</v>
+      </c>
+      <c r="E51" s="337" t="n">
+        <v>43</v>
+      </c>
+      <c r="F51" s="337" t="n">
+        <v>47</v>
+      </c>
+      <c r="G51" s="382" t="n">
+        <v>49</v>
+      </c>
+      <c r="H51" s="382" t="n">
+        <v>52</v>
+      </c>
+      <c r="I51" s="382" t="n">
+        <v>55</v>
+      </c>
+      <c r="J51" s="382" t="n">
+        <v>58</v>
+      </c>
+      <c r="K51" s="382" t="n">
+        <v>61</v>
+      </c>
       <c r="L51" s="186"/>
       <c r="M51" s="186"/>
       <c r="N51" s="186"/>
@@ -19361,20 +19579,36 @@
     </row>
     <row r="52" outlineLevel="1" hidden="0">
       <c r="A52" s="186"/>
-      <c r="B52" s="320" t="s">
+      <c r="B52" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C52" s="320" t="s">
+      <c r="C52" s="323" t="s">
         <v>547</v>
       </c>
-      <c r="D52" s="376"/>
-      <c r="E52" s="376"/>
-      <c r="F52" s="376"/>
-      <c r="G52" s="376"/>
-      <c r="H52" s="376"/>
-      <c r="I52" s="376"/>
-      <c r="J52" s="376"/>
-      <c r="K52" s="376"/>
+      <c r="D52" s="338" t="n">
+        <v>35</v>
+      </c>
+      <c r="E52" s="338" t="n">
+        <v>43</v>
+      </c>
+      <c r="F52" s="338" t="n">
+        <v>47</v>
+      </c>
+      <c r="G52" s="383" t="n">
+        <v>47</v>
+      </c>
+      <c r="H52" s="383" t="n">
+        <v>50</v>
+      </c>
+      <c r="I52" s="383" t="n">
+        <v>53</v>
+      </c>
+      <c r="J52" s="383" t="n">
+        <v>56</v>
+      </c>
+      <c r="K52" s="383" t="n">
+        <v>59</v>
+      </c>
       <c r="L52" s="186"/>
       <c r="M52" s="186"/>
       <c r="N52" s="186"/>
@@ -19387,20 +19621,36 @@
     </row>
     <row r="53" outlineLevel="1" hidden="0">
       <c r="A53" s="186"/>
-      <c r="B53" s="320" t="s">
+      <c r="B53" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C53" s="320" t="s">
+      <c r="C53" s="323" t="s">
         <v>547</v>
       </c>
-      <c r="D53" s="320"/>
-      <c r="E53" s="320"/>
-      <c r="F53" s="377"/>
-      <c r="G53" s="377"/>
-      <c r="H53" s="377"/>
-      <c r="I53" s="377"/>
-      <c r="J53" s="377"/>
-      <c r="K53" s="377"/>
+      <c r="D53" s="384" t="n">
+        <v>35</v>
+      </c>
+      <c r="E53" s="384" t="n">
+        <v>43</v>
+      </c>
+      <c r="F53" s="384" t="n">
+        <v>47</v>
+      </c>
+      <c r="G53" s="384" t="n">
+        <v>49</v>
+      </c>
+      <c r="H53" s="384" t="n">
+        <v>52</v>
+      </c>
+      <c r="I53" s="384" t="n">
+        <v>55</v>
+      </c>
+      <c r="J53" s="384" t="n">
+        <v>58</v>
+      </c>
+      <c r="K53" s="384" t="n">
+        <v>61</v>
+      </c>
       <c r="L53" s="186"/>
       <c r="M53" s="186"/>
       <c r="N53" s="186"/>
@@ -19419,28 +19669,28 @@
       <c r="C54" s="284" t="s">
         <v>551</v>
       </c>
-      <c r="D54" s="320" t="n">
+      <c r="D54" s="385" t="n">
         <v>26.71</v>
       </c>
-      <c r="E54" s="320" t="n">
+      <c r="E54" s="385" t="n">
         <v>29.06</v>
       </c>
-      <c r="F54" s="378" t="n">
+      <c r="F54" s="385" t="n">
         <v>31.41</v>
       </c>
-      <c r="G54" s="378" t="n">
+      <c r="G54" s="385" t="n">
         <v>33.76</v>
       </c>
-      <c r="H54" s="378" t="n">
+      <c r="H54" s="385" t="n">
         <v>36.11</v>
       </c>
-      <c r="I54" s="378" t="n">
+      <c r="I54" s="385" t="n">
         <v>38.46</v>
       </c>
-      <c r="J54" s="378" t="n">
+      <c r="J54" s="385" t="n">
         <v>40.81</v>
       </c>
-      <c r="K54" s="378" t="n">
+      <c r="K54" s="385" t="n">
         <v>43.16</v>
       </c>
       <c r="L54" s="186"/>
@@ -19455,35 +19705,35 @@
     </row>
     <row r="55" outlineLevel="1" hidden="0">
       <c r="A55" s="186"/>
-      <c r="B55" s="320" t="s">
+      <c r="B55" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C55" s="320" t="s">
+      <c r="C55" s="323" t="s">
         <v>551</v>
       </c>
-      <c r="D55" s="320" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="E55" s="320" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="F55" s="379" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="G55" s="379" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="H55" s="379" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="I55" s="379" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="J55" s="379" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="K55" s="379" t="n">
-        <v>26.71</v>
+      <c r="D55" s="386" t="n">
+        <v>73.29</v>
+      </c>
+      <c r="E55" s="386" t="n">
+        <v>70.94</v>
+      </c>
+      <c r="F55" s="386" t="n">
+        <v>68.59</v>
+      </c>
+      <c r="G55" s="386" t="n">
+        <v>66.24</v>
+      </c>
+      <c r="H55" s="386" t="n">
+        <v>63.89</v>
+      </c>
+      <c r="I55" s="386" t="n">
+        <v>61.54</v>
+      </c>
+      <c r="J55" s="386" t="n">
+        <v>59.19</v>
+      </c>
+      <c r="K55" s="386" t="n">
+        <v>56.84</v>
       </c>
       <c r="L55" s="186"/>
       <c r="M55" s="186"/>
@@ -19497,35 +19747,35 @@
     </row>
     <row r="56" outlineLevel="1" hidden="0">
       <c r="A56" s="186"/>
-      <c r="B56" s="320" t="s">
+      <c r="B56" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C56" s="320" t="s">
+      <c r="C56" s="323" t="s">
         <v>551</v>
       </c>
-      <c r="D56" s="320" t="n">
+      <c r="D56" s="323" t="n">
         <v>26.71</v>
       </c>
-      <c r="E56" s="320" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="F56" s="380" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="G56" s="380" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="H56" s="380" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="I56" s="380" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="J56" s="380" t="n">
-        <v>26.71</v>
-      </c>
-      <c r="K56" s="380" t="n">
-        <v>26.71</v>
+      <c r="E56" s="323" t="n">
+        <v>29.06</v>
+      </c>
+      <c r="F56" s="323" t="n">
+        <v>31.41</v>
+      </c>
+      <c r="G56" s="323" t="n">
+        <v>33.76</v>
+      </c>
+      <c r="H56" s="387" t="n">
+        <v>36.11</v>
+      </c>
+      <c r="I56" s="387" t="n">
+        <v>38.46</v>
+      </c>
+      <c r="J56" s="387" t="n">
+        <v>40.81</v>
+      </c>
+      <c r="K56" s="387" t="n">
+        <v>43.16</v>
       </c>
       <c r="L56" s="186"/>
       <c r="M56" s="186"/>
@@ -19543,14 +19793,30 @@
         <v>626</v>
       </c>
       <c r="C57" s="284"/>
-      <c r="D57" s="320"/>
-      <c r="E57" s="320"/>
-      <c r="F57" s="381"/>
-      <c r="G57" s="381"/>
-      <c r="H57" s="381"/>
-      <c r="I57" s="381"/>
-      <c r="J57" s="381"/>
-      <c r="K57" s="381"/>
+      <c r="D57" s="323" t="n">
+        <v>43.3</v>
+      </c>
+      <c r="E57" s="323" t="n">
+        <v>44.54</v>
+      </c>
+      <c r="F57" s="323" t="n">
+        <v>43.79</v>
+      </c>
+      <c r="G57" s="323" t="n">
+        <v>44.45</v>
+      </c>
+      <c r="H57" s="388" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="I57" s="388" t="n">
+        <v>45.4</v>
+      </c>
+      <c r="J57" s="388" t="n">
+        <v>45.89</v>
+      </c>
+      <c r="K57" s="388" t="n">
+        <v>46.39</v>
+      </c>
       <c r="L57" s="186"/>
       <c r="M57" s="186"/>
       <c r="N57" s="186"/>
@@ -19563,18 +19829,34 @@
     </row>
     <row r="58" outlineLevel="1" hidden="0">
       <c r="A58" s="186"/>
-      <c r="B58" s="320" t="s">
+      <c r="B58" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C58" s="320"/>
-      <c r="D58" s="320"/>
-      <c r="E58" s="320"/>
-      <c r="F58" s="382"/>
-      <c r="G58" s="382"/>
-      <c r="H58" s="382"/>
-      <c r="I58" s="382"/>
-      <c r="J58" s="382"/>
-      <c r="K58" s="382"/>
+      <c r="C58" s="323"/>
+      <c r="D58" s="323" t="n">
+        <v>39.02</v>
+      </c>
+      <c r="E58" s="323" t="n">
+        <v>40.17</v>
+      </c>
+      <c r="F58" s="323" t="n">
+        <v>39.34</v>
+      </c>
+      <c r="G58" s="323" t="n">
+        <v>39.32</v>
+      </c>
+      <c r="H58" s="389" t="n">
+        <v>39.52</v>
+      </c>
+      <c r="I58" s="389" t="n">
+        <v>39.76</v>
+      </c>
+      <c r="J58" s="389" t="n">
+        <v>39.99</v>
+      </c>
+      <c r="K58" s="389" t="n">
+        <v>40.23</v>
+      </c>
       <c r="L58" s="186"/>
       <c r="M58" s="186"/>
       <c r="N58" s="186"/>
@@ -19587,18 +19869,34 @@
     </row>
     <row r="59" outlineLevel="1" hidden="0">
       <c r="A59" s="186"/>
-      <c r="B59" s="320" t="s">
+      <c r="B59" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C59" s="320"/>
-      <c r="D59" s="320"/>
-      <c r="E59" s="320"/>
-      <c r="F59" s="320"/>
-      <c r="G59" s="320"/>
-      <c r="H59" s="320"/>
-      <c r="I59" s="320"/>
-      <c r="J59" s="320"/>
-      <c r="K59" s="320"/>
+      <c r="C59" s="323"/>
+      <c r="D59" s="323" t="n">
+        <v>43.3</v>
+      </c>
+      <c r="E59" s="323" t="n">
+        <v>44.54</v>
+      </c>
+      <c r="F59" s="323" t="n">
+        <v>43.79</v>
+      </c>
+      <c r="G59" s="323" t="n">
+        <v>44.45</v>
+      </c>
+      <c r="H59" s="390" t="n">
+        <v>44.87</v>
+      </c>
+      <c r="I59" s="390" t="n">
+        <v>45.4</v>
+      </c>
+      <c r="J59" s="390" t="n">
+        <v>45.89</v>
+      </c>
+      <c r="K59" s="390" t="n">
+        <v>46.39</v>
+      </c>
       <c r="L59" s="186"/>
       <c r="M59" s="186"/>
       <c r="N59" s="186"/>
@@ -19615,14 +19913,30 @@
         <v>626</v>
       </c>
       <c r="C60" s="284"/>
-      <c r="D60" s="320"/>
-      <c r="E60" s="320"/>
-      <c r="F60" s="320"/>
-      <c r="G60" s="320"/>
-      <c r="H60" s="320"/>
-      <c r="I60" s="320"/>
-      <c r="J60" s="320"/>
-      <c r="K60" s="320"/>
+      <c r="D60" s="323" t="n">
+        <v>31.73</v>
+      </c>
+      <c r="E60" s="323" t="n">
+        <v>31.59</v>
+      </c>
+      <c r="F60" s="323" t="n">
+        <v>30.04</v>
+      </c>
+      <c r="G60" s="323" t="n">
+        <v>29.44</v>
+      </c>
+      <c r="H60" s="391" t="n">
+        <v>28.67</v>
+      </c>
+      <c r="I60" s="391" t="n">
+        <v>27.94</v>
+      </c>
+      <c r="J60" s="391" t="n">
+        <v>27.16</v>
+      </c>
+      <c r="K60" s="391" t="n">
+        <v>26.36</v>
+      </c>
       <c r="L60" s="186"/>
       <c r="M60" s="186"/>
       <c r="N60" s="186"/>
@@ -19635,18 +19949,34 @@
     </row>
     <row r="61" outlineLevel="1" hidden="0">
       <c r="A61" s="186"/>
-      <c r="B61" s="320" t="s">
+      <c r="B61" s="323" t="s">
         <v>627</v>
       </c>
-      <c r="C61" s="320"/>
-      <c r="D61" s="320"/>
-      <c r="E61" s="320"/>
-      <c r="F61" s="320"/>
-      <c r="G61" s="320"/>
-      <c r="H61" s="320"/>
-      <c r="I61" s="320"/>
-      <c r="J61" s="320"/>
-      <c r="K61" s="320"/>
+      <c r="C61" s="323"/>
+      <c r="D61" s="323" t="n">
+        <v>10.42</v>
+      </c>
+      <c r="E61" s="323" t="n">
+        <v>11.67</v>
+      </c>
+      <c r="F61" s="323" t="n">
+        <v>12.36</v>
+      </c>
+      <c r="G61" s="323" t="n">
+        <v>13.28</v>
+      </c>
+      <c r="H61" s="392" t="n">
+        <v>14.27</v>
+      </c>
+      <c r="I61" s="392" t="n">
+        <v>15.29</v>
+      </c>
+      <c r="J61" s="392" t="n">
+        <v>16.32</v>
+      </c>
+      <c r="K61" s="392" t="n">
+        <v>17.36</v>
+      </c>
       <c r="L61" s="186"/>
       <c r="M61" s="186"/>
       <c r="N61" s="186"/>
@@ -19659,18 +19989,34 @@
     </row>
     <row r="62" outlineLevel="1" hidden="0">
       <c r="A62" s="186"/>
-      <c r="B62" s="320" t="s">
+      <c r="B62" s="323" t="s">
         <v>628</v>
       </c>
-      <c r="C62" s="320"/>
-      <c r="D62" s="320"/>
-      <c r="E62" s="320"/>
-      <c r="F62" s="320"/>
-      <c r="G62" s="320"/>
-      <c r="H62" s="320"/>
-      <c r="I62" s="320"/>
-      <c r="J62" s="320"/>
-      <c r="K62" s="320"/>
+      <c r="C62" s="323"/>
+      <c r="D62" s="323" t="n">
+        <v>31.73</v>
+      </c>
+      <c r="E62" s="323" t="n">
+        <v>31.59</v>
+      </c>
+      <c r="F62" s="323" t="n">
+        <v>30.04</v>
+      </c>
+      <c r="G62" s="323" t="n">
+        <v>29.44</v>
+      </c>
+      <c r="H62" s="323" t="n">
+        <v>28.67</v>
+      </c>
+      <c r="I62" s="323" t="n">
+        <v>27.94</v>
+      </c>
+      <c r="J62" s="323" t="n">
+        <v>27.16</v>
+      </c>
+      <c r="K62" s="323" t="n">
+        <v>26.36</v>
+      </c>
       <c r="L62" s="186"/>
       <c r="M62" s="186"/>
       <c r="N62" s="186"/>
@@ -21233,66 +21579,66 @@
     <row r="21" ht="33.75" customHeight="1"/>
     <row r="22" ht="162" customHeight="1">
       <c r="B22" s="155"/>
-      <c r="C22" s="386" t="str">
+      <c r="C22" s="396" t="str">
         <f>IF(UHC_Inter!$A3=0,"",UHC_Inter!$A3)</f>
         <v>Demand satisfied with modern methods (married women or in-union) 1</v>
       </c>
-      <c r="D22" s="386" t="str">
+      <c r="D22" s="396" t="str">
         <f>IF(UHC_Inter!$A4=0,"",UHC_Inter!$A4)</f>
         <v>Antenatal care coverage (+4 visits) 2</v>
       </c>
-      <c r="E22" s="386" t="str">
+      <c r="E22" s="396" t="str">
         <f>IF(UHC_Inter!$A5=0,"",UHC_Inter!$A5)</f>
         <v>DPT3 Immunization coverage</v>
       </c>
-      <c r="F22" s="386" t="str">
+      <c r="F22" s="396" t="str">
         <f>IF(UHC_Inter!$A6=0,"",UHC_Inter!$A6)</f>
         <v>Care seeking for suspected pneumonia</v>
       </c>
-      <c r="G22" s="386" t="str">
+      <c r="G22" s="396" t="str">
         <f>IF(UHC_Inter!$A7=0,"",UHC_Inter!$A7)</f>
         <v>TB treatment coverage</v>
       </c>
-      <c r="H22" s="386" t="str">
+      <c r="H22" s="396" t="str">
         <f>IF(UHC_Inter!$A8=0,"",UHC_Inter!$A8)</f>
         <v>HIV ART coverage 4</v>
       </c>
-      <c r="I22" s="386" t="str">
+      <c r="I22" s="396" t="str">
         <f>IF(UHC_Inter!$A9=0,"",UHC_Inter!$A9)</f>
         <v>Use of basic sanitation</v>
       </c>
-      <c r="J22" s="386" t="str">
+      <c r="J22" s="396" t="str">
         <f>IF(UHC_Inter!$A10=0,"",UHC_Inter!$A10)</f>
         <v>Prevalence of raised blood pressure*</v>
       </c>
-      <c r="K22" s="386" t="str">
+      <c r="K22" s="396" t="str">
         <f>IF(UHC_Inter!$A11=0,"",UHC_Inter!$A11)</f>
         <v>Mean fasting blood glucose (mmol/l)*</v>
       </c>
-      <c r="L22" s="386" t="str">
+      <c r="L22" s="396" t="str">
         <f>IF(UHC_Inter!$A12=0,"",UHC_Inter!$A12)</f>
         <v>Tobacco use prevalence* 3</v>
       </c>
-      <c r="M22" s="386" t="str">
+      <c r="M22" s="396" t="str">
         <f>IF(UHC_Inter!$A13=0,"",UHC_Inter!$A13)</f>
         <v>Hospital beds density*</v>
       </c>
-      <c r="N22" s="386" t="str">
+      <c r="N22" s="396" t="str">
         <f>IF(UHC_Inter!$A14=0,"",UHC_Inter!$A14)</f>
         <v>Health worker density*</v>
       </c>
-      <c r="O22" s="386" t="str">
+      <c r="O22" s="396" t="str">
         <f>IF(UHC_Inter!$A15=0,"",UHC_Inter!$A15)</f>
         <v>IHR core capacity index*</v>
       </c>
-      <c r="P22" s="386" t="str">
+      <c r="P22" s="396" t="str">
         <f>IF(UHC_Inter!$A16=0,"",UHC_Inter!$A16)</f>
       </c>
-      <c r="Q22" s="386"/>
-      <c r="R22" s="386"/>
-      <c r="S22" s="386"/>
-      <c r="T22" s="386"/>
-      <c r="U22" s="386"/>
+      <c r="Q22" s="396"/>
+      <c r="R22" s="396"/>
+      <c r="S22" s="396"/>
+      <c r="T22" s="396"/>
+      <c r="U22" s="396"/>
     </row>
     <row r="23">
       <c r="B23" s="111"/>

</xml_diff>